<commit_message>
modify one basis character (빠 -> 뺘)
</commit_message>
<xml_diff>
--- a/output/labels-map(ANSI).xlsx
+++ b/output/labels-map(ANSI).xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="-105" windowWidth="25815" windowHeight="14025" activeTab="1"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="25815" windowHeight="14025" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="labels-map(ANSI)" sheetId="1" r:id="rId1"/>
@@ -7171,10 +7171,6 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>빠</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
     <t>섀</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
@@ -7916,6 +7912,10 @@
   </si>
   <si>
     <t>ㄴ(3)</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>뺘</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
@@ -7923,7 +7923,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="21">
+  <fonts count="23" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -8092,6 +8092,22 @@
     </font>
     <font>
       <sz val="11"/>
+      <name val="맑은 고딕"/>
+      <family val="3"/>
+      <charset val="129"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF00B0F0"/>
+      <name val="맑은 고딕"/>
+      <family val="2"/>
+      <charset val="129"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF00B0F0"/>
       <name val="맑은 고딕"/>
       <family val="3"/>
       <charset val="129"/>
@@ -8556,7 +8572,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -8617,10 +8633,16 @@
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="34" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="34" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="34" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="34" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -8946,15 +8968,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:CV251"/>
   <sheetViews>
-    <sheetView topLeftCell="A169" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="J80" sqref="J80"/>
+    <sheetView topLeftCell="A172" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="S242" sqref="S242"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5"/>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:19">
-      <c r="A1" s="20" t="s">
-        <v>2557</v>
+    <row r="1" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A1" s="23" t="s">
+        <v>2556</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -8984,11 +9006,11 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:19">
-      <c r="A2" s="20"/>
-    </row>
-    <row r="3" spans="1:19">
-      <c r="A3" s="20"/>
+    <row r="2" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A2" s="23"/>
+    </row>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A3" s="23"/>
       <c r="B3" s="2" t="s">
         <v>9</v>
       </c>
@@ -9044,8 +9066,8 @@
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="1:19">
-      <c r="A4" s="20"/>
+    <row r="4" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A4" s="23"/>
       <c r="B4" s="7"/>
       <c r="C4" s="8"/>
       <c r="D4" s="7"/>
@@ -9056,8 +9078,8 @@
       <c r="I4" s="7"/>
       <c r="J4" s="7"/>
     </row>
-    <row r="5" spans="1:19">
-      <c r="A5" s="20"/>
+    <row r="5" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A5" s="23"/>
       <c r="B5" s="2" t="s">
         <v>19</v>
       </c>
@@ -9110,8 +9132,8 @@
         <v>18</v>
       </c>
     </row>
-    <row r="6" spans="1:19">
-      <c r="A6" s="20"/>
+    <row r="6" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A6" s="23"/>
       <c r="B6" s="7"/>
       <c r="C6" s="8"/>
       <c r="D6" s="7"/>
@@ -9122,8 +9144,8 @@
       <c r="I6" s="7"/>
       <c r="J6" s="7"/>
     </row>
-    <row r="7" spans="1:19">
-      <c r="A7" s="20"/>
+    <row r="7" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A7" s="23"/>
       <c r="B7" s="2" t="s">
         <v>27</v>
       </c>
@@ -9176,8 +9198,8 @@
         <v>18</v>
       </c>
     </row>
-    <row r="8" spans="1:19">
-      <c r="A8" s="20"/>
+    <row r="8" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A8" s="23"/>
       <c r="B8" s="7"/>
       <c r="C8" s="8"/>
       <c r="D8" s="7"/>
@@ -9188,8 +9210,8 @@
       <c r="I8" s="7"/>
       <c r="J8" s="7"/>
     </row>
-    <row r="9" spans="1:19">
-      <c r="A9" s="20"/>
+    <row r="9" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A9" s="23"/>
       <c r="B9" s="2" t="s">
         <v>35</v>
       </c>
@@ -9242,8 +9264,8 @@
         <v>18</v>
       </c>
     </row>
-    <row r="10" spans="1:19">
-      <c r="A10" s="20"/>
+    <row r="10" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A10" s="23"/>
       <c r="B10" s="7"/>
       <c r="C10" s="8"/>
       <c r="D10" s="7"/>
@@ -9254,8 +9276,8 @@
       <c r="I10" s="7"/>
       <c r="J10" s="7"/>
     </row>
-    <row r="11" spans="1:19">
-      <c r="A11" s="20"/>
+    <row r="11" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A11" s="23"/>
       <c r="B11" s="2" t="s">
         <v>43</v>
       </c>
@@ -9302,8 +9324,8 @@
         <v>18</v>
       </c>
     </row>
-    <row r="12" spans="1:19">
-      <c r="A12" s="20"/>
+    <row r="12" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A12" s="23"/>
       <c r="B12" s="7"/>
       <c r="C12" s="8"/>
       <c r="D12" s="7"/>
@@ -9314,8 +9336,8 @@
       <c r="I12" s="7"/>
       <c r="J12" s="7"/>
     </row>
-    <row r="13" spans="1:19">
-      <c r="A13" s="20"/>
+    <row r="13" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A13" s="23"/>
       <c r="B13" s="2" t="s">
         <v>49</v>
       </c>
@@ -9368,8 +9390,8 @@
         <v>18</v>
       </c>
     </row>
-    <row r="14" spans="1:19">
-      <c r="A14" s="20"/>
+    <row r="14" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A14" s="23"/>
       <c r="B14" s="7"/>
       <c r="C14" s="8"/>
       <c r="D14" s="7"/>
@@ -9380,8 +9402,8 @@
       <c r="I14" s="7"/>
       <c r="J14" s="7"/>
     </row>
-    <row r="15" spans="1:19">
-      <c r="A15" s="20"/>
+    <row r="15" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A15" s="23"/>
       <c r="B15" s="1" t="s">
         <v>57</v>
       </c>
@@ -9434,8 +9456,8 @@
         <v>18</v>
       </c>
     </row>
-    <row r="16" spans="1:19">
-      <c r="A16" s="20"/>
+    <row r="16" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A16" s="23"/>
       <c r="B16" s="7"/>
       <c r="C16" s="8"/>
       <c r="D16" s="7"/>
@@ -9446,8 +9468,8 @@
       <c r="I16" s="7"/>
       <c r="J16" s="7"/>
     </row>
-    <row r="17" spans="1:19">
-      <c r="A17" s="20"/>
+    <row r="17" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A17" s="23"/>
       <c r="B17" s="2" t="s">
         <v>65</v>
       </c>
@@ -9500,8 +9522,8 @@
         <v>18</v>
       </c>
     </row>
-    <row r="18" spans="1:19">
-      <c r="A18" s="20"/>
+    <row r="18" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A18" s="23"/>
       <c r="B18" s="7"/>
       <c r="C18" s="8"/>
       <c r="D18" s="7"/>
@@ -9512,8 +9534,8 @@
       <c r="I18" s="7"/>
       <c r="J18" s="7"/>
     </row>
-    <row r="19" spans="1:19">
-      <c r="A19" s="20"/>
+    <row r="19" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A19" s="23"/>
       <c r="B19" s="2" t="s">
         <v>73</v>
       </c>
@@ -9563,8 +9585,8 @@
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="1:19">
-      <c r="A20" s="20"/>
+    <row r="20" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A20" s="23"/>
       <c r="B20" s="7"/>
       <c r="C20" s="8"/>
       <c r="D20" s="7"/>
@@ -9575,8 +9597,8 @@
       <c r="I20" s="7"/>
       <c r="J20" s="7"/>
     </row>
-    <row r="21" spans="1:19">
-      <c r="A21" s="20"/>
+    <row r="21" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A21" s="23"/>
       <c r="B21" s="2" t="s">
         <v>80</v>
       </c>
@@ -9632,8 +9654,8 @@
         <v>18</v>
       </c>
     </row>
-    <row r="22" spans="1:19">
-      <c r="A22" s="20"/>
+    <row r="22" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A22" s="23"/>
       <c r="B22" s="7"/>
       <c r="C22" s="8"/>
       <c r="D22" s="7"/>
@@ -9644,8 +9666,8 @@
       <c r="I22" s="7"/>
       <c r="J22" s="7"/>
     </row>
-    <row r="23" spans="1:19">
-      <c r="A23" s="20"/>
+    <row r="23" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A23" s="23"/>
       <c r="B23" s="1" t="s">
         <v>89</v>
       </c>
@@ -9689,8 +9711,8 @@
         <v>18</v>
       </c>
     </row>
-    <row r="24" spans="1:19">
-      <c r="A24" s="20"/>
+    <row r="24" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A24" s="23"/>
       <c r="B24" s="7"/>
       <c r="C24" s="8"/>
       <c r="D24" s="7"/>
@@ -9701,8 +9723,8 @@
       <c r="I24" s="7"/>
       <c r="J24" s="7"/>
     </row>
-    <row r="25" spans="1:19">
-      <c r="A25" s="20"/>
+    <row r="25" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A25" s="23"/>
       <c r="B25" s="2" t="s">
         <v>94</v>
       </c>
@@ -9758,8 +9780,8 @@
         <v>18</v>
       </c>
     </row>
-    <row r="26" spans="1:19">
-      <c r="A26" s="20"/>
+    <row r="26" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A26" s="23"/>
       <c r="B26" s="7"/>
       <c r="C26" s="8"/>
       <c r="D26" s="7"/>
@@ -9770,8 +9792,8 @@
       <c r="I26" s="7"/>
       <c r="J26" s="7"/>
     </row>
-    <row r="27" spans="1:19">
-      <c r="A27" s="20"/>
+    <row r="27" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A27" s="23"/>
       <c r="B27" s="1" t="s">
         <v>103</v>
       </c>
@@ -9827,8 +9849,8 @@
         <v>18</v>
       </c>
     </row>
-    <row r="28" spans="1:19">
-      <c r="A28" s="20"/>
+    <row r="28" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A28" s="23"/>
       <c r="B28" s="7"/>
       <c r="C28" s="8"/>
       <c r="D28" s="7"/>
@@ -9839,8 +9861,8 @@
       <c r="I28" s="7"/>
       <c r="J28" s="7"/>
     </row>
-    <row r="29" spans="1:19">
-      <c r="A29" s="20"/>
+    <row r="29" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A29" s="23"/>
       <c r="B29" s="2" t="s">
         <v>112</v>
       </c>
@@ -9890,8 +9912,8 @@
         <v>18</v>
       </c>
     </row>
-    <row r="30" spans="1:19">
-      <c r="A30" s="20"/>
+    <row r="30" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A30" s="23"/>
       <c r="B30" s="7"/>
       <c r="C30" s="8"/>
       <c r="D30" s="7"/>
@@ -9902,8 +9924,8 @@
       <c r="I30" s="7"/>
       <c r="J30" s="7"/>
     </row>
-    <row r="31" spans="1:19">
-      <c r="A31" s="20"/>
+    <row r="31" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A31" s="23"/>
       <c r="B31" s="2" t="s">
         <v>119</v>
       </c>
@@ -9956,8 +9978,8 @@
         <v>18</v>
       </c>
     </row>
-    <row r="32" spans="1:19">
-      <c r="A32" s="20"/>
+    <row r="32" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A32" s="23"/>
       <c r="B32" s="7"/>
       <c r="C32" s="8"/>
       <c r="D32" s="7"/>
@@ -9968,8 +9990,8 @@
       <c r="I32" s="7"/>
       <c r="J32" s="7"/>
     </row>
-    <row r="33" spans="1:41">
-      <c r="A33" s="20"/>
+    <row r="33" spans="1:41" x14ac:dyDescent="0.3">
+      <c r="A33" s="23"/>
       <c r="B33" s="2" t="s">
         <v>127</v>
       </c>
@@ -10022,8 +10044,8 @@
         <v>18</v>
       </c>
     </row>
-    <row r="34" spans="1:41">
-      <c r="A34" s="20"/>
+    <row r="34" spans="1:41" x14ac:dyDescent="0.3">
+      <c r="A34" s="23"/>
       <c r="B34" s="7"/>
       <c r="C34" s="8"/>
       <c r="D34" s="7"/>
@@ -10034,8 +10056,8 @@
       <c r="I34" s="7"/>
       <c r="J34" s="7"/>
     </row>
-    <row r="35" spans="1:41">
-      <c r="A35" s="20"/>
+    <row r="35" spans="1:41" x14ac:dyDescent="0.3">
+      <c r="A35" s="23"/>
       <c r="B35" s="2" t="s">
         <v>135</v>
       </c>
@@ -10088,8 +10110,8 @@
         <v>18</v>
       </c>
     </row>
-    <row r="36" spans="1:41">
-      <c r="A36" s="20"/>
+    <row r="36" spans="1:41" x14ac:dyDescent="0.3">
+      <c r="A36" s="23"/>
       <c r="B36" s="7"/>
       <c r="C36" s="8"/>
       <c r="D36" s="7"/>
@@ -10100,8 +10122,8 @@
       <c r="I36" s="7"/>
       <c r="J36" s="7"/>
     </row>
-    <row r="37" spans="1:41">
-      <c r="A37" s="20"/>
+    <row r="37" spans="1:41" x14ac:dyDescent="0.3">
+      <c r="A37" s="23"/>
       <c r="B37" s="2" t="s">
         <v>143</v>
       </c>
@@ -10154,8 +10176,8 @@
         <v>18</v>
       </c>
     </row>
-    <row r="38" spans="1:41">
-      <c r="A38" s="20"/>
+    <row r="38" spans="1:41" x14ac:dyDescent="0.3">
+      <c r="A38" s="23"/>
       <c r="B38" s="7"/>
       <c r="C38" s="8"/>
       <c r="D38" s="7"/>
@@ -10166,8 +10188,8 @@
       <c r="I38" s="7"/>
       <c r="J38" s="7"/>
     </row>
-    <row r="39" spans="1:41">
-      <c r="A39" s="20"/>
+    <row r="39" spans="1:41" x14ac:dyDescent="0.3">
+      <c r="A39" s="23"/>
       <c r="B39" s="2" t="s">
         <v>151</v>
       </c>
@@ -10220,8 +10242,8 @@
         <v>18</v>
       </c>
     </row>
-    <row r="40" spans="1:41">
-      <c r="A40" s="20"/>
+    <row r="40" spans="1:41" x14ac:dyDescent="0.3">
+      <c r="A40" s="23"/>
       <c r="B40" s="7"/>
       <c r="C40" s="8"/>
       <c r="D40" s="7"/>
@@ -10232,7 +10254,7 @@
       <c r="I40" s="7"/>
       <c r="J40" s="7"/>
     </row>
-    <row r="41" spans="1:41">
+    <row r="41" spans="1:41" x14ac:dyDescent="0.3">
       <c r="B41" t="s">
         <v>159</v>
       </c>
@@ -10354,10 +10376,13 @@
         <v>159</v>
       </c>
     </row>
-    <row r="43" spans="1:41">
-      <c r="A43" s="20" t="s">
-        <v>2558</v>
-      </c>
+    <row r="42" spans="1:41" x14ac:dyDescent="0.3">
+      <c r="A42" s="23" t="s">
+        <v>2557</v>
+      </c>
+    </row>
+    <row r="43" spans="1:41" x14ac:dyDescent="0.3">
+      <c r="A43" s="23"/>
       <c r="B43" t="s">
         <v>160</v>
       </c>
@@ -10374,11 +10399,11 @@
         <v>164</v>
       </c>
     </row>
-    <row r="44" spans="1:41">
-      <c r="A44" s="20"/>
-    </row>
-    <row r="45" spans="1:41">
-      <c r="A45" s="20"/>
+    <row r="44" spans="1:41" x14ac:dyDescent="0.3">
+      <c r="A44" s="23"/>
+    </row>
+    <row r="45" spans="1:41" x14ac:dyDescent="0.3">
+      <c r="A45" s="23"/>
       <c r="B45" s="2" t="s">
         <v>165</v>
       </c>
@@ -10422,16 +10447,16 @@
         <v>18</v>
       </c>
     </row>
-    <row r="46" spans="1:41">
-      <c r="A46" s="20"/>
+    <row r="46" spans="1:41" x14ac:dyDescent="0.3">
+      <c r="A46" s="23"/>
       <c r="B46" s="7"/>
       <c r="C46" s="7"/>
       <c r="D46" s="7"/>
       <c r="E46" s="7"/>
       <c r="F46" s="7"/>
     </row>
-    <row r="47" spans="1:41">
-      <c r="A47" s="20"/>
+    <row r="47" spans="1:41" x14ac:dyDescent="0.3">
+      <c r="A47" s="23"/>
       <c r="B47" s="2" t="s">
         <v>170</v>
       </c>
@@ -10475,16 +10500,16 @@
         <v>18</v>
       </c>
     </row>
-    <row r="48" spans="1:41">
-      <c r="A48" s="20"/>
+    <row r="48" spans="1:41" x14ac:dyDescent="0.3">
+      <c r="A48" s="23"/>
       <c r="B48" s="7"/>
       <c r="C48" s="7"/>
       <c r="D48" s="7"/>
       <c r="E48" s="7"/>
       <c r="F48" s="7"/>
     </row>
-    <row r="49" spans="1:15">
-      <c r="A49" s="20"/>
+    <row r="49" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A49" s="23"/>
       <c r="B49" s="1" t="s">
         <v>175</v>
       </c>
@@ -10528,16 +10553,16 @@
         <v>18</v>
       </c>
     </row>
-    <row r="50" spans="1:15">
-      <c r="A50" s="20"/>
+    <row r="50" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A50" s="23"/>
       <c r="B50" s="7"/>
       <c r="C50" s="7"/>
       <c r="D50" s="7"/>
       <c r="E50" s="7"/>
       <c r="F50" s="7"/>
     </row>
-    <row r="51" spans="1:15">
-      <c r="A51" s="20"/>
+    <row r="51" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A51" s="23"/>
       <c r="B51" s="2" t="s">
         <v>180</v>
       </c>
@@ -10581,16 +10606,16 @@
         <v>18</v>
       </c>
     </row>
-    <row r="52" spans="1:15">
-      <c r="A52" s="20"/>
+    <row r="52" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A52" s="23"/>
       <c r="B52" s="7"/>
       <c r="C52" s="7"/>
       <c r="D52" s="7"/>
       <c r="E52" s="7"/>
       <c r="F52" s="7"/>
     </row>
-    <row r="53" spans="1:15">
-      <c r="A53" s="20"/>
+    <row r="53" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A53" s="23"/>
       <c r="B53" s="1" t="s">
         <v>185</v>
       </c>
@@ -10628,16 +10653,16 @@
         <v>18</v>
       </c>
     </row>
-    <row r="54" spans="1:15">
-      <c r="A54" s="20"/>
+    <row r="54" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A54" s="23"/>
       <c r="B54" s="7"/>
       <c r="C54" s="7"/>
       <c r="D54" s="7"/>
       <c r="E54" s="7"/>
       <c r="F54" s="7"/>
     </row>
-    <row r="55" spans="1:15">
-      <c r="A55" s="20"/>
+    <row r="55" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A55" s="23"/>
       <c r="B55" s="2" t="s">
         <v>188</v>
       </c>
@@ -10681,16 +10706,16 @@
         <v>18</v>
       </c>
     </row>
-    <row r="56" spans="1:15">
-      <c r="A56" s="20"/>
+    <row r="56" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A56" s="23"/>
       <c r="B56" s="7"/>
       <c r="C56" s="7"/>
       <c r="D56" s="7"/>
       <c r="E56" s="7"/>
       <c r="F56" s="7"/>
     </row>
-    <row r="57" spans="1:15">
-      <c r="A57" s="20"/>
+    <row r="57" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A57" s="23"/>
       <c r="B57" s="2" t="s">
         <v>193</v>
       </c>
@@ -10734,16 +10759,16 @@
         <v>18</v>
       </c>
     </row>
-    <row r="58" spans="1:15">
-      <c r="A58" s="20"/>
+    <row r="58" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A58" s="23"/>
       <c r="B58" s="7"/>
       <c r="C58" s="7"/>
       <c r="D58" s="7"/>
       <c r="E58" s="7"/>
       <c r="F58" s="7"/>
     </row>
-    <row r="59" spans="1:15">
-      <c r="A59" s="20"/>
+    <row r="59" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A59" s="23"/>
       <c r="B59" s="2" t="s">
         <v>198</v>
       </c>
@@ -10787,16 +10812,16 @@
         <v>18</v>
       </c>
     </row>
-    <row r="60" spans="1:15">
-      <c r="A60" s="20"/>
+    <row r="60" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A60" s="23"/>
       <c r="B60" s="7"/>
       <c r="C60" s="7"/>
       <c r="D60" s="7"/>
       <c r="E60" s="7"/>
       <c r="F60" s="7"/>
     </row>
-    <row r="61" spans="1:15">
-      <c r="A61" s="20"/>
+    <row r="61" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A61" s="23"/>
       <c r="B61" s="1" t="s">
         <v>203</v>
       </c>
@@ -10840,16 +10865,16 @@
         <v>18</v>
       </c>
     </row>
-    <row r="62" spans="1:15">
-      <c r="A62" s="20"/>
+    <row r="62" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A62" s="23"/>
       <c r="B62" s="7"/>
       <c r="C62" s="7"/>
       <c r="D62" s="7"/>
       <c r="E62" s="7"/>
       <c r="F62" s="7"/>
     </row>
-    <row r="63" spans="1:15">
-      <c r="A63" s="20"/>
+    <row r="63" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A63" s="23"/>
       <c r="B63" s="2" t="s">
         <v>208</v>
       </c>
@@ -10893,16 +10918,16 @@
         <v>18</v>
       </c>
     </row>
-    <row r="64" spans="1:15">
-      <c r="A64" s="20"/>
+    <row r="64" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A64" s="23"/>
       <c r="B64" s="7"/>
       <c r="C64" s="7"/>
       <c r="D64" s="7"/>
       <c r="E64" s="7"/>
       <c r="F64" s="7"/>
     </row>
-    <row r="65" spans="1:15">
-      <c r="A65" s="20"/>
+    <row r="65" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A65" s="23"/>
       <c r="B65" s="2" t="s">
         <v>213</v>
       </c>
@@ -10943,16 +10968,16 @@
         <v>18</v>
       </c>
     </row>
-    <row r="66" spans="1:15">
-      <c r="A66" s="20"/>
+    <row r="66" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A66" s="23"/>
       <c r="B66" s="7"/>
       <c r="C66" s="7"/>
       <c r="D66" s="7"/>
       <c r="E66" s="7"/>
       <c r="F66" s="7"/>
     </row>
-    <row r="67" spans="1:15">
-      <c r="A67" s="20"/>
+    <row r="67" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A67" s="23"/>
       <c r="B67" s="2" t="s">
         <v>217</v>
       </c>
@@ -10996,16 +11021,16 @@
         <v>18</v>
       </c>
     </row>
-    <row r="68" spans="1:15">
-      <c r="A68" s="20"/>
+    <row r="68" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A68" s="23"/>
       <c r="B68" s="7"/>
       <c r="C68" s="7"/>
       <c r="D68" s="7"/>
       <c r="E68" s="7"/>
       <c r="F68" s="7"/>
     </row>
-    <row r="69" spans="1:15">
-      <c r="A69" s="20"/>
+    <row r="69" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A69" s="23"/>
       <c r="B69" s="2" t="s">
         <v>222</v>
       </c>
@@ -11049,16 +11074,16 @@
         <v>18</v>
       </c>
     </row>
-    <row r="70" spans="1:15">
-      <c r="A70" s="20"/>
+    <row r="70" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A70" s="23"/>
       <c r="B70" s="7"/>
       <c r="C70" s="7"/>
       <c r="D70" s="7"/>
       <c r="E70" s="7"/>
       <c r="F70" s="7"/>
     </row>
-    <row r="71" spans="1:15">
-      <c r="A71" s="20"/>
+    <row r="71" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A71" s="23"/>
       <c r="B71" s="2" t="s">
         <v>227</v>
       </c>
@@ -11099,16 +11124,16 @@
         <v>18</v>
       </c>
     </row>
-    <row r="72" spans="1:15">
-      <c r="A72" s="20"/>
+    <row r="72" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A72" s="23"/>
       <c r="B72" s="7"/>
       <c r="C72" s="7"/>
       <c r="D72" s="7"/>
       <c r="E72" s="7"/>
       <c r="F72" s="7"/>
     </row>
-    <row r="73" spans="1:15">
-      <c r="A73" s="20"/>
+    <row r="73" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A73" s="23"/>
       <c r="B73" s="2" t="s">
         <v>231</v>
       </c>
@@ -11152,16 +11177,16 @@
         <v>18</v>
       </c>
     </row>
-    <row r="74" spans="1:15">
-      <c r="A74" s="20"/>
+    <row r="74" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A74" s="23"/>
       <c r="B74" s="7"/>
       <c r="C74" s="7"/>
       <c r="D74" s="7"/>
       <c r="E74" s="7"/>
       <c r="F74" s="7"/>
     </row>
-    <row r="75" spans="1:15">
-      <c r="A75" s="20"/>
+    <row r="75" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A75" s="23"/>
       <c r="B75" s="1" t="s">
         <v>236</v>
       </c>
@@ -11205,16 +11230,16 @@
         <v>18</v>
       </c>
     </row>
-    <row r="76" spans="1:15">
-      <c r="A76" s="20"/>
+    <row r="76" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A76" s="23"/>
       <c r="B76" s="7"/>
       <c r="C76" s="7"/>
       <c r="D76" s="7"/>
       <c r="E76" s="7"/>
       <c r="F76" s="7"/>
     </row>
-    <row r="77" spans="1:15">
-      <c r="A77" s="20"/>
+    <row r="77" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A77" s="23"/>
       <c r="B77" s="2" t="s">
         <v>241</v>
       </c>
@@ -11258,16 +11283,16 @@
         <v>18</v>
       </c>
     </row>
-    <row r="78" spans="1:15">
-      <c r="A78" s="20"/>
+    <row r="78" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A78" s="23"/>
       <c r="B78" s="7"/>
       <c r="C78" s="7"/>
       <c r="D78" s="7"/>
       <c r="E78" s="7"/>
       <c r="F78" s="7"/>
     </row>
-    <row r="79" spans="1:15">
-      <c r="A79" s="20"/>
+    <row r="79" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A79" s="23"/>
       <c r="B79" s="2" t="s">
         <v>246</v>
       </c>
@@ -11311,16 +11336,16 @@
         <v>18</v>
       </c>
     </row>
-    <row r="80" spans="1:15">
-      <c r="A80" s="20"/>
+    <row r="80" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A80" s="23"/>
       <c r="B80" s="7"/>
       <c r="C80" s="7"/>
       <c r="D80" s="7"/>
       <c r="E80" s="7"/>
       <c r="F80" s="7"/>
     </row>
-    <row r="81" spans="1:41">
-      <c r="A81" s="20"/>
+    <row r="81" spans="1:41" x14ac:dyDescent="0.3">
+      <c r="A81" s="23"/>
       <c r="B81" s="2" t="s">
         <v>251</v>
       </c>
@@ -11364,15 +11389,15 @@
         <v>18</v>
       </c>
     </row>
-    <row r="82" spans="1:41">
-      <c r="A82" s="20"/>
+    <row r="82" spans="1:41" x14ac:dyDescent="0.3">
+      <c r="A82" s="23"/>
       <c r="B82" s="7"/>
       <c r="C82" s="7"/>
       <c r="D82" s="7"/>
       <c r="E82" s="7"/>
       <c r="F82" s="7"/>
     </row>
-    <row r="83" spans="1:41">
+    <row r="83" spans="1:41" x14ac:dyDescent="0.3">
       <c r="B83" t="s">
         <v>159</v>
       </c>
@@ -11494,10 +11519,13 @@
         <v>159</v>
       </c>
     </row>
-    <row r="85" spans="1:41">
-      <c r="A85" s="20" t="s">
-        <v>2559</v>
-      </c>
+    <row r="84" spans="1:41" x14ac:dyDescent="0.3">
+      <c r="A84" s="23" t="s">
+        <v>2558</v>
+      </c>
+    </row>
+    <row r="85" spans="1:41" x14ac:dyDescent="0.3">
+      <c r="A85" s="23"/>
       <c r="B85" t="s">
         <v>256</v>
       </c>
@@ -11520,11 +11548,11 @@
         <v>262</v>
       </c>
     </row>
-    <row r="86" spans="1:41">
-      <c r="A86" s="20"/>
-    </row>
-    <row r="87" spans="1:41">
-      <c r="A87" s="20"/>
+    <row r="86" spans="1:41" x14ac:dyDescent="0.3">
+      <c r="A86" s="23"/>
+    </row>
+    <row r="87" spans="1:41" x14ac:dyDescent="0.3">
+      <c r="A87" s="23"/>
       <c r="B87" s="2" t="s">
         <v>263</v>
       </c>
@@ -11574,8 +11602,8 @@
         <v>18</v>
       </c>
     </row>
-    <row r="88" spans="1:41">
-      <c r="A88" s="20"/>
+    <row r="88" spans="1:41" x14ac:dyDescent="0.3">
+      <c r="A88" s="23"/>
       <c r="B88" s="7"/>
       <c r="C88" s="7"/>
       <c r="D88" s="7"/>
@@ -11584,8 +11612,8 @@
       <c r="G88" s="7"/>
       <c r="H88" s="7"/>
     </row>
-    <row r="89" spans="1:41">
-      <c r="A89" s="20"/>
+    <row r="89" spans="1:41" x14ac:dyDescent="0.3">
+      <c r="A89" s="23"/>
       <c r="B89" s="2" t="s">
         <v>270</v>
       </c>
@@ -11593,7 +11621,7 @@
         <v>271</v>
       </c>
       <c r="D89" s="2" t="s">
-        <v>2484</v>
+        <v>2483</v>
       </c>
       <c r="E89" s="2" t="s">
         <v>272</v>
@@ -11632,8 +11660,8 @@
         <v>18</v>
       </c>
     </row>
-    <row r="90" spans="1:41">
-      <c r="A90" s="20"/>
+    <row r="90" spans="1:41" x14ac:dyDescent="0.3">
+      <c r="A90" s="23"/>
       <c r="B90" s="7"/>
       <c r="C90" s="7"/>
       <c r="D90" s="7"/>
@@ -11642,8 +11670,8 @@
       <c r="G90" s="7"/>
       <c r="H90" s="7"/>
     </row>
-    <row r="91" spans="1:41">
-      <c r="A91" s="20"/>
+    <row r="91" spans="1:41" x14ac:dyDescent="0.3">
+      <c r="A91" s="23"/>
       <c r="B91" s="2" t="s">
         <v>275</v>
       </c>
@@ -11690,8 +11718,8 @@
         <v>18</v>
       </c>
     </row>
-    <row r="92" spans="1:41">
-      <c r="A92" s="20"/>
+    <row r="92" spans="1:41" x14ac:dyDescent="0.3">
+      <c r="A92" s="23"/>
       <c r="B92" s="7"/>
       <c r="C92" s="7"/>
       <c r="D92" s="7"/>
@@ -11700,8 +11728,8 @@
       <c r="G92" s="7"/>
       <c r="H92" s="7"/>
     </row>
-    <row r="93" spans="1:41">
-      <c r="A93" s="20"/>
+    <row r="93" spans="1:41" x14ac:dyDescent="0.3">
+      <c r="A93" s="23"/>
       <c r="B93" s="1" t="s">
         <v>281</v>
       </c>
@@ -11751,8 +11779,8 @@
         <v>18</v>
       </c>
     </row>
-    <row r="94" spans="1:41">
-      <c r="A94" s="20"/>
+    <row r="94" spans="1:41" x14ac:dyDescent="0.3">
+      <c r="A94" s="23"/>
       <c r="B94" s="7"/>
       <c r="C94" s="7"/>
       <c r="D94" s="7"/>
@@ -11761,8 +11789,8 @@
       <c r="G94" s="7"/>
       <c r="H94" s="7"/>
     </row>
-    <row r="95" spans="1:41">
-      <c r="A95" s="20"/>
+    <row r="95" spans="1:41" x14ac:dyDescent="0.3">
+      <c r="A95" s="23"/>
       <c r="B95" s="1" t="s">
         <v>288</v>
       </c>
@@ -11809,8 +11837,8 @@
         <v>18</v>
       </c>
     </row>
-    <row r="96" spans="1:41">
-      <c r="A96" s="20"/>
+    <row r="96" spans="1:41" x14ac:dyDescent="0.3">
+      <c r="A96" s="23"/>
       <c r="B96" s="7"/>
       <c r="C96" s="7"/>
       <c r="D96" s="7"/>
@@ -11819,8 +11847,8 @@
       <c r="G96" s="7"/>
       <c r="H96" s="7"/>
     </row>
-    <row r="97" spans="1:17">
-      <c r="A97" s="20"/>
+    <row r="97" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A97" s="23"/>
       <c r="B97" s="2" t="s">
         <v>294</v>
       </c>
@@ -11864,8 +11892,8 @@
         <v>18</v>
       </c>
     </row>
-    <row r="98" spans="1:17">
-      <c r="A98" s="20"/>
+    <row r="98" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A98" s="23"/>
       <c r="B98" s="7"/>
       <c r="C98" s="7"/>
       <c r="D98" s="7"/>
@@ -11874,8 +11902,8 @@
       <c r="G98" s="7"/>
       <c r="H98" s="7"/>
     </row>
-    <row r="99" spans="1:17">
-      <c r="A99" s="20"/>
+    <row r="99" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A99" s="23"/>
       <c r="B99" s="2" t="s">
         <v>299</v>
       </c>
@@ -11919,8 +11947,8 @@
         <v>18</v>
       </c>
     </row>
-    <row r="100" spans="1:17">
-      <c r="A100" s="20"/>
+    <row r="100" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A100" s="23"/>
       <c r="B100" s="7"/>
       <c r="C100" s="7"/>
       <c r="D100" s="7"/>
@@ -11929,8 +11957,8 @@
       <c r="G100" s="7"/>
       <c r="H100" s="7"/>
     </row>
-    <row r="101" spans="1:17">
-      <c r="A101" s="20"/>
+    <row r="101" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A101" s="23"/>
       <c r="B101" s="2" t="s">
         <v>304</v>
       </c>
@@ -11977,8 +12005,8 @@
         <v>18</v>
       </c>
     </row>
-    <row r="102" spans="1:17">
-      <c r="A102" s="20"/>
+    <row r="102" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A102" s="23"/>
       <c r="B102" s="7"/>
       <c r="C102" s="7"/>
       <c r="D102" s="7"/>
@@ -11987,8 +12015,8 @@
       <c r="G102" s="7"/>
       <c r="H102" s="7"/>
     </row>
-    <row r="103" spans="1:17">
-      <c r="A103" s="20"/>
+    <row r="103" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A103" s="23"/>
       <c r="B103" s="2" t="s">
         <v>18</v>
       </c>
@@ -12020,8 +12048,8 @@
         <v>18</v>
       </c>
     </row>
-    <row r="104" spans="1:17">
-      <c r="A104" s="20"/>
+    <row r="104" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A104" s="23"/>
       <c r="B104" s="7"/>
       <c r="C104" s="7"/>
       <c r="D104" s="7"/>
@@ -12030,8 +12058,8 @@
       <c r="G104" s="7"/>
       <c r="H104" s="7"/>
     </row>
-    <row r="105" spans="1:17">
-      <c r="A105" s="20"/>
+    <row r="105" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A105" s="23"/>
       <c r="B105" s="2" t="s">
         <v>311</v>
       </c>
@@ -12078,8 +12106,8 @@
         <v>18</v>
       </c>
     </row>
-    <row r="106" spans="1:17">
-      <c r="A106" s="20"/>
+    <row r="106" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A106" s="23"/>
       <c r="B106" s="7"/>
       <c r="C106" s="7"/>
       <c r="D106" s="7"/>
@@ -12088,8 +12116,8 @@
       <c r="G106" s="7"/>
       <c r="H106" s="7"/>
     </row>
-    <row r="107" spans="1:17">
-      <c r="A107" s="20"/>
+    <row r="107" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A107" s="23"/>
       <c r="B107" s="2" t="s">
         <v>317</v>
       </c>
@@ -12139,8 +12167,8 @@
         <v>18</v>
       </c>
     </row>
-    <row r="108" spans="1:17">
-      <c r="A108" s="20"/>
+    <row r="108" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A108" s="23"/>
       <c r="B108" s="7"/>
       <c r="C108" s="7"/>
       <c r="D108" s="7"/>
@@ -12149,8 +12177,8 @@
       <c r="G108" s="7"/>
       <c r="H108" s="7"/>
     </row>
-    <row r="109" spans="1:17">
-      <c r="A109" s="20"/>
+    <row r="109" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A109" s="23"/>
       <c r="B109" s="2" t="s">
         <v>324</v>
       </c>
@@ -12200,8 +12228,8 @@
         <v>18</v>
       </c>
     </row>
-    <row r="110" spans="1:17">
-      <c r="A110" s="20"/>
+    <row r="110" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A110" s="23"/>
       <c r="B110" s="7"/>
       <c r="C110" s="7"/>
       <c r="D110" s="7"/>
@@ -12210,8 +12238,8 @@
       <c r="G110" s="7"/>
       <c r="H110" s="7"/>
     </row>
-    <row r="111" spans="1:17">
-      <c r="A111" s="20"/>
+    <row r="111" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A111" s="23"/>
       <c r="B111" s="2" t="s">
         <v>331</v>
       </c>
@@ -12258,8 +12286,8 @@
         <v>18</v>
       </c>
     </row>
-    <row r="112" spans="1:17">
-      <c r="A112" s="20"/>
+    <row r="112" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A112" s="23"/>
       <c r="B112" s="7"/>
       <c r="C112" s="7"/>
       <c r="D112" s="7"/>
@@ -12268,8 +12296,8 @@
       <c r="G112" s="7"/>
       <c r="H112" s="7"/>
     </row>
-    <row r="113" spans="1:41">
-      <c r="A113" s="20"/>
+    <row r="113" spans="1:41" x14ac:dyDescent="0.3">
+      <c r="A113" s="23"/>
       <c r="B113" s="2" t="s">
         <v>337</v>
       </c>
@@ -12313,8 +12341,8 @@
         <v>18</v>
       </c>
     </row>
-    <row r="114" spans="1:41">
-      <c r="A114" s="20"/>
+    <row r="114" spans="1:41" x14ac:dyDescent="0.3">
+      <c r="A114" s="23"/>
       <c r="B114" s="7"/>
       <c r="C114" s="7"/>
       <c r="D114" s="7"/>
@@ -12323,8 +12351,8 @@
       <c r="G114" s="7"/>
       <c r="H114" s="7"/>
     </row>
-    <row r="115" spans="1:41">
-      <c r="A115" s="20"/>
+    <row r="115" spans="1:41" x14ac:dyDescent="0.3">
+      <c r="A115" s="23"/>
       <c r="B115" s="2" t="s">
         <v>342</v>
       </c>
@@ -12368,8 +12396,8 @@
         <v>18</v>
       </c>
     </row>
-    <row r="116" spans="1:41">
-      <c r="A116" s="20"/>
+    <row r="116" spans="1:41" x14ac:dyDescent="0.3">
+      <c r="A116" s="23"/>
       <c r="B116" s="7"/>
       <c r="C116" s="7"/>
       <c r="D116" s="7"/>
@@ -12378,8 +12406,8 @@
       <c r="G116" s="7"/>
       <c r="H116" s="7"/>
     </row>
-    <row r="117" spans="1:41">
-      <c r="A117" s="20"/>
+    <row r="117" spans="1:41" x14ac:dyDescent="0.3">
+      <c r="A117" s="23"/>
       <c r="B117" s="2" t="s">
         <v>347</v>
       </c>
@@ -12426,8 +12454,8 @@
         <v>18</v>
       </c>
     </row>
-    <row r="118" spans="1:41">
-      <c r="A118" s="20"/>
+    <row r="118" spans="1:41" x14ac:dyDescent="0.3">
+      <c r="A118" s="23"/>
       <c r="B118" s="7"/>
       <c r="C118" s="7"/>
       <c r="D118" s="7"/>
@@ -12436,8 +12464,8 @@
       <c r="G118" s="7"/>
       <c r="H118" s="7"/>
     </row>
-    <row r="119" spans="1:41">
-      <c r="A119" s="20"/>
+    <row r="119" spans="1:41" x14ac:dyDescent="0.3">
+      <c r="A119" s="23"/>
       <c r="B119" s="2" t="s">
         <v>353</v>
       </c>
@@ -12487,8 +12515,8 @@
         <v>18</v>
       </c>
     </row>
-    <row r="120" spans="1:41">
-      <c r="A120" s="20"/>
+    <row r="120" spans="1:41" x14ac:dyDescent="0.3">
+      <c r="A120" s="23"/>
       <c r="B120" s="7"/>
       <c r="C120" s="7"/>
       <c r="D120" s="7"/>
@@ -12497,8 +12525,8 @@
       <c r="G120" s="7"/>
       <c r="H120" s="7"/>
     </row>
-    <row r="121" spans="1:41">
-      <c r="A121" s="20"/>
+    <row r="121" spans="1:41" x14ac:dyDescent="0.3">
+      <c r="A121" s="23"/>
       <c r="B121" s="1" t="s">
         <v>360</v>
       </c>
@@ -12539,8 +12567,8 @@
         <v>18</v>
       </c>
     </row>
-    <row r="122" spans="1:41">
-      <c r="A122" s="20"/>
+    <row r="122" spans="1:41" x14ac:dyDescent="0.3">
+      <c r="A122" s="23"/>
       <c r="B122" s="7"/>
       <c r="C122" s="7"/>
       <c r="D122" s="7"/>
@@ -12549,8 +12577,8 @@
       <c r="G122" s="7"/>
       <c r="H122" s="7"/>
     </row>
-    <row r="123" spans="1:41">
-      <c r="A123" s="20"/>
+    <row r="123" spans="1:41" x14ac:dyDescent="0.3">
+      <c r="A123" s="23"/>
       <c r="B123" s="2" t="s">
         <v>364</v>
       </c>
@@ -12600,8 +12628,8 @@
         <v>18</v>
       </c>
     </row>
-    <row r="124" spans="1:41">
-      <c r="A124" s="20"/>
+    <row r="124" spans="1:41" x14ac:dyDescent="0.3">
+      <c r="A124" s="23"/>
       <c r="B124" s="7"/>
       <c r="C124" s="7"/>
       <c r="D124" s="7"/>
@@ -12610,7 +12638,7 @@
       <c r="G124" s="7"/>
       <c r="H124" s="7"/>
     </row>
-    <row r="125" spans="1:41">
+    <row r="125" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A125" s="18"/>
       <c r="B125" t="s">
         <v>159</v>
@@ -12733,13 +12761,13 @@
         <v>159</v>
       </c>
     </row>
-    <row r="126" spans="1:41">
-      <c r="A126" s="18"/>
-    </row>
-    <row r="127" spans="1:41">
-      <c r="A127" s="20" t="s">
-        <v>2563</v>
-      </c>
+    <row r="126" spans="1:41" x14ac:dyDescent="0.3">
+      <c r="A126" s="23" t="s">
+        <v>2562</v>
+      </c>
+    </row>
+    <row r="127" spans="1:41" x14ac:dyDescent="0.3">
+      <c r="A127" s="23"/>
       <c r="B127" t="s">
         <v>0</v>
       </c>
@@ -12773,11 +12801,11 @@
       <c r="N127" s="7"/>
       <c r="O127" s="7"/>
     </row>
-    <row r="128" spans="1:41">
-      <c r="A128" s="20"/>
-    </row>
-    <row r="129" spans="1:100">
-      <c r="A129" s="20"/>
+    <row r="128" spans="1:41" x14ac:dyDescent="0.3">
+      <c r="A128" s="23"/>
+    </row>
+    <row r="129" spans="1:100" x14ac:dyDescent="0.3">
+      <c r="A129" s="23"/>
       <c r="B129" s="2" t="s">
         <v>371</v>
       </c>
@@ -13036,8 +13064,8 @@
       <c r="CU129" s="7"/>
       <c r="CV129" s="7"/>
     </row>
-    <row r="130" spans="1:100">
-      <c r="A130" s="20"/>
+    <row r="130" spans="1:100" x14ac:dyDescent="0.3">
+      <c r="A130" s="23"/>
       <c r="B130" s="7"/>
       <c r="C130" s="7"/>
       <c r="D130" s="7"/>
@@ -13138,8 +13166,8 @@
       <c r="CU130" s="7"/>
       <c r="CV130" s="7"/>
     </row>
-    <row r="131" spans="1:100">
-      <c r="A131" s="20"/>
+    <row r="131" spans="1:100" x14ac:dyDescent="0.3">
+      <c r="A131" s="23"/>
       <c r="B131" s="2" t="s">
         <v>450</v>
       </c>
@@ -13334,8 +13362,8 @@
       <c r="CU131" s="7"/>
       <c r="CV131" s="7"/>
     </row>
-    <row r="132" spans="1:100">
-      <c r="A132" s="20"/>
+    <row r="132" spans="1:100" x14ac:dyDescent="0.3">
+      <c r="A132" s="23"/>
       <c r="B132" s="7"/>
       <c r="C132" s="7"/>
       <c r="D132" s="7"/>
@@ -13436,8 +13464,8 @@
       <c r="CU132" s="7"/>
       <c r="CV132" s="7"/>
     </row>
-    <row r="133" spans="1:100">
-      <c r="A133" s="20"/>
+    <row r="133" spans="1:100" x14ac:dyDescent="0.3">
+      <c r="A133" s="23"/>
       <c r="B133" s="2" t="s">
         <v>497</v>
       </c>
@@ -13672,8 +13700,8 @@
       <c r="CU133" s="7"/>
       <c r="CV133" s="7"/>
     </row>
-    <row r="134" spans="1:100">
-      <c r="A134" s="20"/>
+    <row r="134" spans="1:100" x14ac:dyDescent="0.3">
+      <c r="A134" s="23"/>
       <c r="B134" s="7"/>
       <c r="C134" s="7"/>
       <c r="D134" s="7"/>
@@ -13774,8 +13802,8 @@
       <c r="CU134" s="7"/>
       <c r="CV134" s="7"/>
     </row>
-    <row r="135" spans="1:100">
-      <c r="A135" s="20"/>
+    <row r="135" spans="1:100" x14ac:dyDescent="0.3">
+      <c r="A135" s="23"/>
       <c r="B135" s="2" t="s">
         <v>564</v>
       </c>
@@ -13998,8 +14026,8 @@
       <c r="CU135" s="7"/>
       <c r="CV135" s="7"/>
     </row>
-    <row r="136" spans="1:100">
-      <c r="A136" s="20"/>
+    <row r="136" spans="1:100" x14ac:dyDescent="0.3">
+      <c r="A136" s="23"/>
       <c r="B136" s="7"/>
       <c r="C136" s="7"/>
       <c r="D136" s="7"/>
@@ -14100,8 +14128,8 @@
       <c r="CU136" s="7"/>
       <c r="CV136" s="7"/>
     </row>
-    <row r="137" spans="1:100">
-      <c r="A137" s="20"/>
+    <row r="137" spans="1:100" x14ac:dyDescent="0.3">
+      <c r="A137" s="23"/>
       <c r="B137" s="2" t="s">
         <v>625</v>
       </c>
@@ -14288,8 +14316,8 @@
       <c r="CU137" s="7"/>
       <c r="CV137" s="7"/>
     </row>
-    <row r="138" spans="1:100">
-      <c r="A138" s="20"/>
+    <row r="138" spans="1:100" x14ac:dyDescent="0.3">
+      <c r="A138" s="23"/>
       <c r="B138" s="7"/>
       <c r="C138" s="7"/>
       <c r="D138" s="7"/>
@@ -14390,8 +14418,8 @@
       <c r="CU138" s="7"/>
       <c r="CV138" s="7"/>
     </row>
-    <row r="139" spans="1:100">
-      <c r="A139" s="20"/>
+    <row r="139" spans="1:100" x14ac:dyDescent="0.3">
+      <c r="A139" s="23"/>
       <c r="B139" s="2" t="s">
         <v>667</v>
       </c>
@@ -14606,8 +14634,8 @@
       <c r="CU139" s="7"/>
       <c r="CV139" s="7"/>
     </row>
-    <row r="140" spans="1:100">
-      <c r="A140" s="20"/>
+    <row r="140" spans="1:100" x14ac:dyDescent="0.3">
+      <c r="A140" s="23"/>
       <c r="B140" s="7"/>
       <c r="C140" s="7"/>
       <c r="D140" s="7"/>
@@ -14708,8 +14736,8 @@
       <c r="CU140" s="7"/>
       <c r="CV140" s="7"/>
     </row>
-    <row r="141" spans="1:100">
-      <c r="A141" s="20"/>
+    <row r="141" spans="1:100" x14ac:dyDescent="0.3">
+      <c r="A141" s="23"/>
       <c r="B141" s="2" t="s">
         <v>724</v>
       </c>
@@ -14936,8 +14964,8 @@
       <c r="CU141" s="7"/>
       <c r="CV141" s="7"/>
     </row>
-    <row r="142" spans="1:100">
-      <c r="A142" s="20"/>
+    <row r="142" spans="1:100" x14ac:dyDescent="0.3">
+      <c r="A142" s="23"/>
       <c r="B142" s="7"/>
       <c r="C142" s="7"/>
       <c r="D142" s="7"/>
@@ -15038,8 +15066,8 @@
       <c r="CU142" s="7"/>
       <c r="CV142" s="7"/>
     </row>
-    <row r="143" spans="1:100">
-      <c r="A143" s="20"/>
+    <row r="143" spans="1:100" x14ac:dyDescent="0.3">
+      <c r="A143" s="23"/>
       <c r="B143" s="2" t="s">
         <v>787</v>
       </c>
@@ -15268,8 +15296,8 @@
       <c r="CU143" s="7"/>
       <c r="CV143" s="7"/>
     </row>
-    <row r="144" spans="1:100">
-      <c r="A144" s="20"/>
+    <row r="144" spans="1:100" x14ac:dyDescent="0.3">
+      <c r="A144" s="23"/>
       <c r="B144" s="7"/>
       <c r="C144" s="7"/>
       <c r="D144" s="7"/>
@@ -15370,8 +15398,8 @@
       <c r="CU144" s="7"/>
       <c r="CV144" s="7"/>
     </row>
-    <row r="145" spans="1:100">
-      <c r="A145" s="20"/>
+    <row r="145" spans="1:100" x14ac:dyDescent="0.3">
+      <c r="A145" s="23"/>
       <c r="B145" s="2" t="s">
         <v>851</v>
       </c>
@@ -15556,8 +15584,8 @@
       <c r="CU145" s="7"/>
       <c r="CV145" s="7"/>
     </row>
-    <row r="146" spans="1:100">
-      <c r="A146" s="20"/>
+    <row r="146" spans="1:100" x14ac:dyDescent="0.3">
+      <c r="A146" s="23"/>
       <c r="B146" s="7"/>
       <c r="C146" s="7"/>
       <c r="D146" s="7"/>
@@ -15658,8 +15686,8 @@
       <c r="CU146" s="7"/>
       <c r="CV146" s="7"/>
     </row>
-    <row r="147" spans="1:100">
-      <c r="A147" s="20"/>
+    <row r="147" spans="1:100" x14ac:dyDescent="0.3">
+      <c r="A147" s="23"/>
       <c r="B147" s="2" t="s">
         <v>893</v>
       </c>
@@ -15910,8 +15938,8 @@
       <c r="CU147" s="7"/>
       <c r="CV147" s="7"/>
     </row>
-    <row r="148" spans="1:100">
-      <c r="A148" s="20"/>
+    <row r="148" spans="1:100" x14ac:dyDescent="0.3">
+      <c r="A148" s="23"/>
       <c r="B148" s="7"/>
       <c r="C148" s="7"/>
       <c r="D148" s="7"/>
@@ -16012,8 +16040,8 @@
       <c r="CU148" s="7"/>
       <c r="CV148" s="7"/>
     </row>
-    <row r="149" spans="1:100">
-      <c r="A149" s="20"/>
+    <row r="149" spans="1:100" x14ac:dyDescent="0.3">
+      <c r="A149" s="23"/>
       <c r="B149" s="2" t="s">
         <v>968</v>
       </c>
@@ -16184,8 +16212,8 @@
       <c r="CU149" s="7"/>
       <c r="CV149" s="7"/>
     </row>
-    <row r="150" spans="1:100">
-      <c r="A150" s="20"/>
+    <row r="150" spans="1:100" x14ac:dyDescent="0.3">
+      <c r="A150" s="23"/>
       <c r="B150" s="7"/>
       <c r="C150" s="7"/>
       <c r="D150" s="7"/>
@@ -16286,8 +16314,8 @@
       <c r="CU150" s="7"/>
       <c r="CV150" s="7"/>
     </row>
-    <row r="151" spans="1:100">
-      <c r="A151" s="20"/>
+    <row r="151" spans="1:100" x14ac:dyDescent="0.3">
+      <c r="A151" s="23"/>
       <c r="B151" s="2" t="s">
         <v>1003</v>
       </c>
@@ -16572,8 +16600,8 @@
       <c r="CU151" s="7"/>
       <c r="CV151" s="7"/>
     </row>
-    <row r="152" spans="1:100">
-      <c r="A152" s="20"/>
+    <row r="152" spans="1:100" x14ac:dyDescent="0.3">
+      <c r="A152" s="23"/>
       <c r="B152" s="7"/>
       <c r="C152" s="7"/>
       <c r="D152" s="7"/>
@@ -16674,8 +16702,8 @@
       <c r="CU152" s="7"/>
       <c r="CV152" s="7"/>
     </row>
-    <row r="153" spans="1:100">
-      <c r="A153" s="20"/>
+    <row r="153" spans="1:100" x14ac:dyDescent="0.3">
+      <c r="A153" s="23"/>
       <c r="B153" s="2" t="s">
         <v>1095</v>
       </c>
@@ -16900,8 +16928,8 @@
       <c r="CU153" s="7"/>
       <c r="CV153" s="7"/>
     </row>
-    <row r="154" spans="1:100">
-      <c r="A154" s="20"/>
+    <row r="154" spans="1:100" x14ac:dyDescent="0.3">
+      <c r="A154" s="23"/>
       <c r="B154" s="7"/>
       <c r="C154" s="7"/>
       <c r="D154" s="7"/>
@@ -17002,8 +17030,8 @@
       <c r="CU154" s="7"/>
       <c r="CV154" s="7"/>
     </row>
-    <row r="155" spans="1:100">
-      <c r="A155" s="20"/>
+    <row r="155" spans="1:100" x14ac:dyDescent="0.3">
+      <c r="A155" s="23"/>
       <c r="B155" s="2" t="s">
         <v>1157</v>
       </c>
@@ -17180,8 +17208,8 @@
       <c r="CU155" s="7"/>
       <c r="CV155" s="7"/>
     </row>
-    <row r="156" spans="1:100">
-      <c r="A156" s="20"/>
+    <row r="156" spans="1:100" x14ac:dyDescent="0.3">
+      <c r="A156" s="23"/>
       <c r="B156" s="7"/>
       <c r="C156" s="7"/>
       <c r="D156" s="7"/>
@@ -17281,8 +17309,8 @@
       <c r="CU156" s="7"/>
       <c r="CV156" s="7"/>
     </row>
-    <row r="157" spans="1:100">
-      <c r="A157" s="20"/>
+    <row r="157" spans="1:100" x14ac:dyDescent="0.3">
+      <c r="A157" s="23"/>
       <c r="B157" s="2" t="s">
         <v>1195</v>
       </c>
@@ -17485,8 +17513,8 @@
       <c r="CU157" s="7"/>
       <c r="CV157" s="7"/>
     </row>
-    <row r="158" spans="1:100">
-      <c r="A158" s="20"/>
+    <row r="158" spans="1:100" x14ac:dyDescent="0.3">
+      <c r="A158" s="23"/>
       <c r="B158" s="7"/>
       <c r="C158" s="7"/>
       <c r="D158" s="7"/>
@@ -17587,8 +17615,8 @@
       <c r="CU158" s="7"/>
       <c r="CV158" s="7"/>
     </row>
-    <row r="159" spans="1:100">
-      <c r="A159" s="20"/>
+    <row r="159" spans="1:100" x14ac:dyDescent="0.3">
+      <c r="A159" s="23"/>
       <c r="B159" s="2" t="s">
         <v>1246</v>
       </c>
@@ -17783,8 +17811,8 @@
       <c r="CU159" s="7"/>
       <c r="CV159" s="7"/>
     </row>
-    <row r="160" spans="1:100">
-      <c r="A160" s="20"/>
+    <row r="160" spans="1:100" x14ac:dyDescent="0.3">
+      <c r="A160" s="23"/>
       <c r="B160" s="7"/>
       <c r="C160" s="7"/>
       <c r="D160" s="7"/>
@@ -17885,8 +17913,8 @@
       <c r="CU160" s="7"/>
       <c r="CV160" s="7"/>
     </row>
-    <row r="161" spans="1:100">
-      <c r="A161" s="20"/>
+    <row r="161" spans="1:100" x14ac:dyDescent="0.3">
+      <c r="A161" s="23"/>
       <c r="B161" s="2" t="s">
         <v>1293</v>
       </c>
@@ -18075,8 +18103,8 @@
       <c r="CU161" s="7"/>
       <c r="CV161" s="7"/>
     </row>
-    <row r="162" spans="1:100">
-      <c r="A162" s="20"/>
+    <row r="162" spans="1:100" x14ac:dyDescent="0.3">
+      <c r="A162" s="23"/>
       <c r="B162" s="7"/>
       <c r="C162" s="7"/>
       <c r="D162" s="7"/>
@@ -18177,8 +18205,8 @@
       <c r="CU162" s="7"/>
       <c r="CV162" s="7"/>
     </row>
-    <row r="163" spans="1:100">
-      <c r="A163" s="20"/>
+    <row r="163" spans="1:100" x14ac:dyDescent="0.3">
+      <c r="A163" s="23"/>
       <c r="B163" s="2" t="s">
         <v>1337</v>
       </c>
@@ -18381,8 +18409,8 @@
       <c r="CU163" s="7"/>
       <c r="CV163" s="7"/>
     </row>
-    <row r="164" spans="1:100">
-      <c r="A164" s="20"/>
+    <row r="164" spans="1:100" x14ac:dyDescent="0.3">
+      <c r="A164" s="23"/>
       <c r="B164" s="7"/>
       <c r="C164" s="7"/>
       <c r="D164" s="7"/>
@@ -18483,8 +18511,8 @@
       <c r="CU164" s="7"/>
       <c r="CV164" s="7"/>
     </row>
-    <row r="165" spans="1:100">
-      <c r="A165" s="20"/>
+    <row r="165" spans="1:100" x14ac:dyDescent="0.3">
+      <c r="A165" s="23"/>
       <c r="B165" s="2" t="s">
         <v>1388</v>
       </c>
@@ -18685,8 +18713,8 @@
       <c r="CU165" s="7"/>
       <c r="CV165" s="7"/>
     </row>
-    <row r="166" spans="1:100">
-      <c r="A166" s="20"/>
+    <row r="166" spans="1:100" x14ac:dyDescent="0.3">
+      <c r="A166" s="23"/>
       <c r="B166" s="7"/>
       <c r="C166" s="7"/>
       <c r="D166" s="7"/>
@@ -18782,7 +18810,7 @@
       <c r="CP166" s="7"/>
       <c r="CQ166" s="7"/>
     </row>
-    <row r="167" spans="1:100">
+    <row r="167" spans="1:100" x14ac:dyDescent="0.3">
       <c r="B167" t="s">
         <v>159</v>
       </c>
@@ -18904,10 +18932,13 @@
         <v>159</v>
       </c>
     </row>
-    <row r="169" spans="1:100">
-      <c r="A169" s="20" t="s">
-        <v>2561</v>
-      </c>
+    <row r="168" spans="1:100" x14ac:dyDescent="0.3">
+      <c r="A168" s="23" t="s">
+        <v>2560</v>
+      </c>
+    </row>
+    <row r="169" spans="1:100" x14ac:dyDescent="0.3">
+      <c r="A169" s="23"/>
       <c r="B169" t="s">
         <v>160</v>
       </c>
@@ -18930,11 +18961,11 @@
       <c r="K169" s="7"/>
       <c r="L169" s="7"/>
     </row>
-    <row r="170" spans="1:100">
-      <c r="A170" s="20"/>
-    </row>
-    <row r="171" spans="1:100">
-      <c r="A171" s="20"/>
+    <row r="170" spans="1:100" x14ac:dyDescent="0.3">
+      <c r="A170" s="23"/>
+    </row>
+    <row r="171" spans="1:100" x14ac:dyDescent="0.3">
+      <c r="A171" s="23"/>
       <c r="B171" s="2" t="s">
         <v>1438</v>
       </c>
@@ -19068,8 +19099,8 @@
       <c r="BB171" s="7"/>
       <c r="BC171" s="7"/>
     </row>
-    <row r="172" spans="1:100">
-      <c r="A172" s="20"/>
+    <row r="172" spans="1:100" x14ac:dyDescent="0.3">
+      <c r="A172" s="23"/>
       <c r="B172" s="7"/>
       <c r="C172" s="7"/>
       <c r="D172" s="7"/>
@@ -19125,8 +19156,8 @@
       <c r="BB172" s="7"/>
       <c r="BC172" s="7"/>
     </row>
-    <row r="173" spans="1:100">
-      <c r="A173" s="20"/>
+    <row r="173" spans="1:100" x14ac:dyDescent="0.3">
+      <c r="A173" s="23"/>
       <c r="B173" s="2" t="s">
         <v>1477</v>
       </c>
@@ -19244,8 +19275,8 @@
       <c r="BD173" s="7"/>
       <c r="BE173" s="7"/>
     </row>
-    <row r="174" spans="1:100">
-      <c r="A174" s="20"/>
+    <row r="174" spans="1:100" x14ac:dyDescent="0.3">
+      <c r="A174" s="23"/>
       <c r="B174" s="7"/>
       <c r="C174" s="7"/>
       <c r="D174" s="7"/>
@@ -19303,8 +19334,8 @@
       <c r="BD174" s="7"/>
       <c r="BE174" s="7"/>
     </row>
-    <row r="175" spans="1:100">
-      <c r="A175" s="20"/>
+    <row r="175" spans="1:100" x14ac:dyDescent="0.3">
+      <c r="A175" s="23"/>
       <c r="B175" s="2" t="s">
         <v>1506</v>
       </c>
@@ -19442,8 +19473,8 @@
       <c r="BD175" s="7"/>
       <c r="BE175" s="7"/>
     </row>
-    <row r="176" spans="1:100">
-      <c r="A176" s="20"/>
+    <row r="176" spans="1:100" x14ac:dyDescent="0.3">
+      <c r="A176" s="23"/>
       <c r="B176" s="7"/>
       <c r="C176" s="7"/>
       <c r="D176" s="7"/>
@@ -19501,8 +19532,8 @@
       <c r="BD176" s="7"/>
       <c r="BE176" s="7"/>
     </row>
-    <row r="177" spans="1:57">
-      <c r="A177" s="20"/>
+    <row r="177" spans="1:57" x14ac:dyDescent="0.3">
+      <c r="A177" s="23"/>
       <c r="B177" s="2" t="s">
         <v>1546</v>
       </c>
@@ -19624,8 +19655,8 @@
       <c r="BD177" s="7"/>
       <c r="BE177" s="7"/>
     </row>
-    <row r="178" spans="1:57">
-      <c r="A178" s="20"/>
+    <row r="178" spans="1:57" x14ac:dyDescent="0.3">
+      <c r="A178" s="23"/>
       <c r="B178" s="7"/>
       <c r="C178" s="7"/>
       <c r="D178" s="7"/>
@@ -19683,8 +19714,8 @@
       <c r="BD178" s="7"/>
       <c r="BE178" s="7"/>
     </row>
-    <row r="179" spans="1:57">
-      <c r="A179" s="20"/>
+    <row r="179" spans="1:57" x14ac:dyDescent="0.3">
+      <c r="A179" s="23"/>
       <c r="B179" s="2" t="s">
         <v>1578</v>
       </c>
@@ -19776,8 +19807,8 @@
       <c r="BD179" s="7"/>
       <c r="BE179" s="7"/>
     </row>
-    <row r="180" spans="1:57">
-      <c r="A180" s="20"/>
+    <row r="180" spans="1:57" x14ac:dyDescent="0.3">
+      <c r="A180" s="23"/>
       <c r="B180" s="7"/>
       <c r="C180" s="7"/>
       <c r="D180" s="7"/>
@@ -19835,8 +19866,8 @@
       <c r="BD180" s="7"/>
       <c r="BE180" s="7"/>
     </row>
-    <row r="181" spans="1:57">
-      <c r="A181" s="20"/>
+    <row r="181" spans="1:57" x14ac:dyDescent="0.3">
+      <c r="A181" s="23"/>
       <c r="B181" s="2" t="s">
         <v>1595</v>
       </c>
@@ -19966,8 +19997,8 @@
       <c r="BD181" s="7"/>
       <c r="BE181" s="7"/>
     </row>
-    <row r="182" spans="1:57">
-      <c r="A182" s="20"/>
+    <row r="182" spans="1:57" x14ac:dyDescent="0.3">
+      <c r="A182" s="23"/>
       <c r="B182" s="7"/>
       <c r="C182" s="7"/>
       <c r="D182" s="7"/>
@@ -20025,8 +20056,8 @@
       <c r="BD182" s="7"/>
       <c r="BE182" s="7"/>
     </row>
-    <row r="183" spans="1:57">
-      <c r="A183" s="20"/>
+    <row r="183" spans="1:57" x14ac:dyDescent="0.3">
+      <c r="A183" s="23"/>
       <c r="B183" s="2" t="s">
         <v>1631</v>
       </c>
@@ -20152,8 +20183,8 @@
       <c r="BD183" s="7"/>
       <c r="BE183" s="7"/>
     </row>
-    <row r="184" spans="1:57">
-      <c r="A184" s="20"/>
+    <row r="184" spans="1:57" x14ac:dyDescent="0.3">
+      <c r="A184" s="23"/>
       <c r="B184" s="7"/>
       <c r="C184" s="7"/>
       <c r="D184" s="7"/>
@@ -20211,8 +20242,8 @@
       <c r="BD184" s="7"/>
       <c r="BE184" s="7"/>
     </row>
-    <row r="185" spans="1:57">
-      <c r="A185" s="20"/>
+    <row r="185" spans="1:57" x14ac:dyDescent="0.3">
+      <c r="A185" s="23"/>
       <c r="B185" s="2" t="s">
         <v>1665</v>
       </c>
@@ -20334,8 +20365,8 @@
       <c r="BD185" s="7"/>
       <c r="BE185" s="7"/>
     </row>
-    <row r="186" spans="1:57">
-      <c r="A186" s="20"/>
+    <row r="186" spans="1:57" x14ac:dyDescent="0.3">
+      <c r="A186" s="23"/>
       <c r="B186" s="7"/>
       <c r="C186" s="7"/>
       <c r="D186" s="7"/>
@@ -20393,8 +20424,8 @@
       <c r="BD186" s="7"/>
       <c r="BE186" s="7"/>
     </row>
-    <row r="187" spans="1:57">
-      <c r="A187" s="20"/>
+    <row r="187" spans="1:57" x14ac:dyDescent="0.3">
+      <c r="A187" s="23"/>
       <c r="B187" s="2" t="s">
         <v>1697</v>
       </c>
@@ -20488,8 +20519,8 @@
       <c r="BD187" s="7"/>
       <c r="BE187" s="7"/>
     </row>
-    <row r="188" spans="1:57">
-      <c r="A188" s="20"/>
+    <row r="188" spans="1:57" x14ac:dyDescent="0.3">
+      <c r="A188" s="23"/>
       <c r="B188" s="7"/>
       <c r="C188" s="7"/>
       <c r="D188" s="7"/>
@@ -20547,8 +20578,8 @@
       <c r="BD188" s="7"/>
       <c r="BE188" s="7"/>
     </row>
-    <row r="189" spans="1:57">
-      <c r="A189" s="20"/>
+    <row r="189" spans="1:57" x14ac:dyDescent="0.3">
+      <c r="A189" s="23"/>
       <c r="B189" s="2" t="s">
         <v>1715</v>
       </c>
@@ -20688,8 +20719,8 @@
       <c r="BD189" s="7"/>
       <c r="BE189" s="7"/>
     </row>
-    <row r="190" spans="1:57">
-      <c r="A190" s="20"/>
+    <row r="190" spans="1:57" x14ac:dyDescent="0.3">
+      <c r="A190" s="23"/>
       <c r="B190" s="7"/>
       <c r="C190" s="7"/>
       <c r="D190" s="7"/>
@@ -20747,8 +20778,8 @@
       <c r="BD190" s="7"/>
       <c r="BE190" s="7"/>
     </row>
-    <row r="191" spans="1:57">
-      <c r="A191" s="20"/>
+    <row r="191" spans="1:57" x14ac:dyDescent="0.3">
+      <c r="A191" s="23"/>
       <c r="B191" s="2" t="s">
         <v>1756</v>
       </c>
@@ -20850,8 +20881,8 @@
       <c r="BD191" s="7"/>
       <c r="BE191" s="7"/>
     </row>
-    <row r="192" spans="1:57">
-      <c r="A192" s="20"/>
+    <row r="192" spans="1:57" x14ac:dyDescent="0.3">
+      <c r="A192" s="23"/>
       <c r="B192" s="7"/>
       <c r="C192" s="7"/>
       <c r="D192" s="7"/>
@@ -20909,8 +20940,8 @@
       <c r="BD192" s="7"/>
       <c r="BE192" s="7"/>
     </row>
-    <row r="193" spans="1:57">
-      <c r="A193" s="20"/>
+    <row r="193" spans="1:57" x14ac:dyDescent="0.3">
+      <c r="A193" s="23"/>
       <c r="B193" s="2" t="s">
         <v>1778</v>
       </c>
@@ -21068,8 +21099,8 @@
       <c r="BD193" s="7"/>
       <c r="BE193" s="7"/>
     </row>
-    <row r="194" spans="1:57">
-      <c r="A194" s="20"/>
+    <row r="194" spans="1:57" x14ac:dyDescent="0.3">
+      <c r="A194" s="23"/>
       <c r="B194" s="7"/>
       <c r="C194" s="7"/>
       <c r="D194" s="7"/>
@@ -21127,8 +21158,8 @@
       <c r="BD194" s="7"/>
       <c r="BE194" s="7"/>
     </row>
-    <row r="195" spans="1:57">
-      <c r="A195" s="20"/>
+    <row r="195" spans="1:57" x14ac:dyDescent="0.3">
+      <c r="A195" s="23"/>
       <c r="B195" s="2" t="s">
         <v>1828</v>
       </c>
@@ -21252,8 +21283,8 @@
       <c r="BD195" s="7"/>
       <c r="BE195" s="7"/>
     </row>
-    <row r="196" spans="1:57">
-      <c r="A196" s="20"/>
+    <row r="196" spans="1:57" x14ac:dyDescent="0.3">
+      <c r="A196" s="23"/>
       <c r="B196" s="7"/>
       <c r="C196" s="7"/>
       <c r="D196" s="7"/>
@@ -21311,8 +21342,8 @@
       <c r="BD196" s="7"/>
       <c r="BE196" s="7"/>
     </row>
-    <row r="197" spans="1:57">
-      <c r="A197" s="20"/>
+    <row r="197" spans="1:57" x14ac:dyDescent="0.3">
+      <c r="A197" s="23"/>
       <c r="B197" s="2" t="s">
         <v>1861</v>
       </c>
@@ -21406,8 +21437,8 @@
       <c r="BD197" s="7"/>
       <c r="BE197" s="7"/>
     </row>
-    <row r="198" spans="1:57">
-      <c r="A198" s="20"/>
+    <row r="198" spans="1:57" x14ac:dyDescent="0.3">
+      <c r="A198" s="23"/>
       <c r="B198" s="7"/>
       <c r="C198" s="7"/>
       <c r="D198" s="7"/>
@@ -21465,8 +21496,8 @@
       <c r="BD198" s="7"/>
       <c r="BE198" s="7"/>
     </row>
-    <row r="199" spans="1:57">
-      <c r="A199" s="20"/>
+    <row r="199" spans="1:57" x14ac:dyDescent="0.3">
+      <c r="A199" s="23"/>
       <c r="B199" s="2" t="s">
         <v>1879</v>
       </c>
@@ -21576,8 +21607,8 @@
       <c r="BD199" s="7"/>
       <c r="BE199" s="7"/>
     </row>
-    <row r="200" spans="1:57">
-      <c r="A200" s="20"/>
+    <row r="200" spans="1:57" x14ac:dyDescent="0.3">
+      <c r="A200" s="23"/>
       <c r="B200" s="7"/>
       <c r="C200" s="7"/>
       <c r="D200" s="7"/>
@@ -21635,8 +21666,8 @@
       <c r="BD200" s="7"/>
       <c r="BE200" s="7"/>
     </row>
-    <row r="201" spans="1:57">
-      <c r="A201" s="20"/>
+    <row r="201" spans="1:57" x14ac:dyDescent="0.3">
+      <c r="A201" s="23"/>
       <c r="B201" s="2" t="s">
         <v>1905</v>
       </c>
@@ -21740,8 +21771,8 @@
       <c r="BD201" s="7"/>
       <c r="BE201" s="7"/>
     </row>
-    <row r="202" spans="1:57">
-      <c r="A202" s="20"/>
+    <row r="202" spans="1:57" x14ac:dyDescent="0.3">
+      <c r="A202" s="23"/>
       <c r="B202" s="7"/>
       <c r="C202" s="7"/>
       <c r="D202" s="7"/>
@@ -21799,8 +21830,8 @@
       <c r="BD202" s="7"/>
       <c r="BE202" s="7"/>
     </row>
-    <row r="203" spans="1:57">
-      <c r="A203" s="20"/>
+    <row r="203" spans="1:57" x14ac:dyDescent="0.3">
+      <c r="A203" s="23"/>
       <c r="B203" s="2" t="s">
         <v>1928</v>
       </c>
@@ -21912,8 +21943,8 @@
       <c r="BD203" s="7"/>
       <c r="BE203" s="7"/>
     </row>
-    <row r="204" spans="1:57">
-      <c r="A204" s="20"/>
+    <row r="204" spans="1:57" x14ac:dyDescent="0.3">
+      <c r="A204" s="23"/>
       <c r="B204" s="7"/>
       <c r="C204" s="7"/>
       <c r="D204" s="7"/>
@@ -21971,8 +22002,8 @@
       <c r="BD204" s="7"/>
       <c r="BE204" s="7"/>
     </row>
-    <row r="205" spans="1:57">
-      <c r="A205" s="20"/>
+    <row r="205" spans="1:57" x14ac:dyDescent="0.3">
+      <c r="A205" s="23"/>
       <c r="B205" s="2" t="s">
         <v>1955</v>
       </c>
@@ -22090,8 +22121,8 @@
       <c r="BD205" s="7"/>
       <c r="BE205" s="7"/>
     </row>
-    <row r="206" spans="1:57">
-      <c r="A206" s="20"/>
+    <row r="206" spans="1:57" x14ac:dyDescent="0.3">
+      <c r="A206" s="23"/>
       <c r="B206" s="7"/>
       <c r="C206" s="7"/>
       <c r="D206" s="7"/>
@@ -22149,8 +22180,8 @@
       <c r="BD206" s="7"/>
       <c r="BE206" s="7"/>
     </row>
-    <row r="207" spans="1:57">
-      <c r="A207" s="20"/>
+    <row r="207" spans="1:57" x14ac:dyDescent="0.3">
+      <c r="A207" s="23"/>
       <c r="B207" s="2" t="s">
         <v>1985</v>
       </c>
@@ -22282,8 +22313,8 @@
       <c r="BD207" s="7"/>
       <c r="BE207" s="7"/>
     </row>
-    <row r="208" spans="1:57">
-      <c r="A208" s="20"/>
+    <row r="208" spans="1:57" x14ac:dyDescent="0.3">
+      <c r="A208" s="23"/>
       <c r="B208" s="7"/>
       <c r="C208" s="7"/>
       <c r="D208" s="7"/>
@@ -22341,7 +22372,7 @@
       <c r="BD208" s="7"/>
       <c r="BE208" s="7"/>
     </row>
-    <row r="209" spans="1:57">
+    <row r="209" spans="1:57" x14ac:dyDescent="0.3">
       <c r="B209" s="7" t="s">
         <v>159</v>
       </c>
@@ -22479,10 +22510,13 @@
       <c r="BD209" s="7"/>
       <c r="BE209" s="7"/>
     </row>
-    <row r="211" spans="1:57">
-      <c r="A211" s="20" t="s">
-        <v>2562</v>
-      </c>
+    <row r="210" spans="1:57" x14ac:dyDescent="0.3">
+      <c r="A210" s="23" t="s">
+        <v>2561</v>
+      </c>
+    </row>
+    <row r="211" spans="1:57" x14ac:dyDescent="0.3">
+      <c r="A211" s="23"/>
       <c r="B211" t="s">
         <v>256</v>
       </c>
@@ -22505,11 +22539,11 @@
         <v>262</v>
       </c>
     </row>
-    <row r="212" spans="1:57">
-      <c r="A212" s="20"/>
-    </row>
-    <row r="213" spans="1:57">
-      <c r="A213" s="20"/>
+    <row r="212" spans="1:57" x14ac:dyDescent="0.3">
+      <c r="A212" s="23"/>
+    </row>
+    <row r="213" spans="1:57" x14ac:dyDescent="0.3">
+      <c r="A213" s="23"/>
       <c r="B213" s="2" t="s">
         <v>2022</v>
       </c>
@@ -22618,8 +22652,8 @@
       <c r="AQ213" s="7"/>
       <c r="AR213" s="7"/>
     </row>
-    <row r="214" spans="1:57">
-      <c r="A214" s="20"/>
+    <row r="214" spans="1:57" x14ac:dyDescent="0.3">
+      <c r="A214" s="23"/>
       <c r="B214" s="7"/>
       <c r="C214" s="7"/>
       <c r="D214" s="7"/>
@@ -22664,8 +22698,8 @@
       <c r="AQ214" s="7"/>
       <c r="AR214" s="7"/>
     </row>
-    <row r="215" spans="1:57">
-      <c r="A215" s="20"/>
+    <row r="215" spans="1:57" x14ac:dyDescent="0.3">
+      <c r="A215" s="23"/>
       <c r="B215" s="2" t="s">
         <v>2054</v>
       </c>
@@ -22758,8 +22792,8 @@
       <c r="AQ215" s="7"/>
       <c r="AR215" s="7"/>
     </row>
-    <row r="216" spans="1:57">
-      <c r="A216" s="20"/>
+    <row r="216" spans="1:57" x14ac:dyDescent="0.3">
+      <c r="A216" s="23"/>
       <c r="B216" s="7"/>
       <c r="C216" s="7"/>
       <c r="D216" s="7"/>
@@ -22804,8 +22838,8 @@
       <c r="AQ216" s="7"/>
       <c r="AR216" s="7"/>
     </row>
-    <row r="217" spans="1:57">
-      <c r="A217" s="20"/>
+    <row r="217" spans="1:57" x14ac:dyDescent="0.3">
+      <c r="A217" s="23"/>
       <c r="B217" s="2" t="s">
         <v>2078</v>
       </c>
@@ -22880,8 +22914,8 @@
       <c r="AQ217" s="7"/>
       <c r="AR217" s="7"/>
     </row>
-    <row r="218" spans="1:57">
-      <c r="A218" s="20"/>
+    <row r="218" spans="1:57" x14ac:dyDescent="0.3">
+      <c r="A218" s="23"/>
       <c r="B218" s="7"/>
       <c r="C218" s="7"/>
       <c r="D218" s="7"/>
@@ -22926,8 +22960,8 @@
       <c r="AQ218" s="7"/>
       <c r="AR218" s="7"/>
     </row>
-    <row r="219" spans="1:57">
-      <c r="A219" s="20"/>
+    <row r="219" spans="1:57" x14ac:dyDescent="0.3">
+      <c r="A219" s="23"/>
       <c r="B219" s="2" t="s">
         <v>2093</v>
       </c>
@@ -23002,8 +23036,8 @@
       <c r="AQ219" s="7"/>
       <c r="AR219" s="7"/>
     </row>
-    <row r="220" spans="1:57">
-      <c r="A220" s="20"/>
+    <row r="220" spans="1:57" x14ac:dyDescent="0.3">
+      <c r="A220" s="23"/>
       <c r="B220" s="7"/>
       <c r="C220" s="7"/>
       <c r="D220" s="7"/>
@@ -23048,8 +23082,8 @@
       <c r="AQ220" s="7"/>
       <c r="AR220" s="7"/>
     </row>
-    <row r="221" spans="1:57">
-      <c r="A221" s="20"/>
+    <row r="221" spans="1:57" x14ac:dyDescent="0.3">
+      <c r="A221" s="23"/>
       <c r="B221" s="2" t="s">
         <v>2108</v>
       </c>
@@ -23116,8 +23150,8 @@
       <c r="AQ221" s="7"/>
       <c r="AR221" s="7"/>
     </row>
-    <row r="222" spans="1:57">
-      <c r="A222" s="20"/>
+    <row r="222" spans="1:57" x14ac:dyDescent="0.3">
+      <c r="A222" s="23"/>
       <c r="B222" s="7"/>
       <c r="C222" s="7"/>
       <c r="D222" s="7"/>
@@ -23162,8 +23196,8 @@
       <c r="AQ222" s="7"/>
       <c r="AR222" s="7"/>
     </row>
-    <row r="223" spans="1:57">
-      <c r="A223" s="20"/>
+    <row r="223" spans="1:57" x14ac:dyDescent="0.3">
+      <c r="A223" s="23"/>
       <c r="B223" s="2" t="s">
         <v>2119</v>
       </c>
@@ -23240,8 +23274,8 @@
       <c r="AQ223" s="7"/>
       <c r="AR223" s="7"/>
     </row>
-    <row r="224" spans="1:57">
-      <c r="A224" s="20"/>
+    <row r="224" spans="1:57" x14ac:dyDescent="0.3">
+      <c r="A224" s="23"/>
       <c r="B224" s="7"/>
       <c r="C224" s="7"/>
       <c r="D224" s="7"/>
@@ -23286,8 +23320,8 @@
       <c r="AQ224" s="7"/>
       <c r="AR224" s="7"/>
     </row>
-    <row r="225" spans="1:45">
-      <c r="A225" s="20"/>
+    <row r="225" spans="1:45" x14ac:dyDescent="0.3">
+      <c r="A225" s="23"/>
       <c r="B225" s="2" t="s">
         <v>2135</v>
       </c>
@@ -23360,8 +23394,8 @@
       <c r="AQ225" s="7"/>
       <c r="AR225" s="7"/>
     </row>
-    <row r="226" spans="1:45">
-      <c r="A226" s="20"/>
+    <row r="226" spans="1:45" x14ac:dyDescent="0.3">
+      <c r="A226" s="23"/>
       <c r="B226" s="7"/>
       <c r="C226" s="7"/>
       <c r="D226" s="7"/>
@@ -23406,8 +23440,8 @@
       <c r="AQ226" s="7"/>
       <c r="AR226" s="7"/>
     </row>
-    <row r="227" spans="1:45">
-      <c r="A227" s="20"/>
+    <row r="227" spans="1:45" x14ac:dyDescent="0.3">
+      <c r="A227" s="23"/>
       <c r="B227" s="2" t="s">
         <v>2149</v>
       </c>
@@ -23480,8 +23514,8 @@
       <c r="AQ227" s="7"/>
       <c r="AR227" s="7"/>
     </row>
-    <row r="228" spans="1:45">
-      <c r="A228" s="20"/>
+    <row r="228" spans="1:45" x14ac:dyDescent="0.3">
+      <c r="A228" s="23"/>
       <c r="B228" s="7"/>
       <c r="C228" s="7"/>
       <c r="D228" s="7"/>
@@ -23526,8 +23560,8 @@
       <c r="AQ228" s="7"/>
       <c r="AR228" s="7"/>
     </row>
-    <row r="229" spans="1:45">
-      <c r="A229" s="20"/>
+    <row r="229" spans="1:45" x14ac:dyDescent="0.3">
+      <c r="A229" s="23"/>
       <c r="B229" s="7"/>
       <c r="C229" s="7"/>
       <c r="D229" s="7"/>
@@ -23572,8 +23606,8 @@
       <c r="AQ229" s="7"/>
       <c r="AR229" s="7"/>
     </row>
-    <row r="230" spans="1:45">
-      <c r="A230" s="20"/>
+    <row r="230" spans="1:45" x14ac:dyDescent="0.3">
+      <c r="A230" s="23"/>
       <c r="B230" s="7"/>
       <c r="C230" s="7"/>
       <c r="D230" s="7"/>
@@ -23618,8 +23652,8 @@
       <c r="AQ230" s="7"/>
       <c r="AR230" s="7"/>
     </row>
-    <row r="231" spans="1:45">
-      <c r="A231" s="20"/>
+    <row r="231" spans="1:45" x14ac:dyDescent="0.3">
+      <c r="A231" s="23"/>
       <c r="B231" s="2" t="s">
         <v>2163</v>
       </c>
@@ -23718,8 +23752,8 @@
       <c r="AQ231" s="7"/>
       <c r="AR231" s="7"/>
     </row>
-    <row r="232" spans="1:45">
-      <c r="A232" s="20"/>
+    <row r="232" spans="1:45" x14ac:dyDescent="0.3">
+      <c r="A232" s="23"/>
       <c r="B232" s="7"/>
       <c r="C232" s="7"/>
       <c r="D232" s="7"/>
@@ -23764,8 +23798,8 @@
       <c r="AQ232" s="7"/>
       <c r="AR232" s="7"/>
     </row>
-    <row r="233" spans="1:45">
-      <c r="A233" s="20"/>
+    <row r="233" spans="1:45" x14ac:dyDescent="0.3">
+      <c r="A233" s="23"/>
       <c r="B233" s="2" t="s">
         <v>2190</v>
       </c>
@@ -23836,8 +23870,8 @@
       <c r="AQ233" s="7"/>
       <c r="AR233" s="7"/>
     </row>
-    <row r="234" spans="1:45">
-      <c r="A234" s="20"/>
+    <row r="234" spans="1:45" x14ac:dyDescent="0.3">
+      <c r="A234" s="23"/>
       <c r="B234" s="7"/>
       <c r="C234" s="7"/>
       <c r="D234" s="7"/>
@@ -23882,8 +23916,8 @@
       <c r="AQ234" s="7"/>
       <c r="AR234" s="7"/>
     </row>
-    <row r="235" spans="1:45">
-      <c r="A235" s="20"/>
+    <row r="235" spans="1:45" x14ac:dyDescent="0.3">
+      <c r="A235" s="23"/>
       <c r="B235" s="2" t="s">
         <v>2202</v>
       </c>
@@ -24017,8 +24051,8 @@
         <v>2245</v>
       </c>
     </row>
-    <row r="236" spans="1:45">
-      <c r="A236" s="20"/>
+    <row r="236" spans="1:45" x14ac:dyDescent="0.3">
+      <c r="A236" s="23"/>
       <c r="B236" s="7"/>
       <c r="C236" s="7"/>
       <c r="D236" s="7"/>
@@ -24063,8 +24097,8 @@
       <c r="AQ236" s="7"/>
       <c r="AR236" s="7"/>
     </row>
-    <row r="237" spans="1:45">
-      <c r="A237" s="20"/>
+    <row r="237" spans="1:45" x14ac:dyDescent="0.3">
+      <c r="A237" s="23"/>
       <c r="B237" s="2" t="s">
         <v>2246</v>
       </c>
@@ -24149,8 +24183,8 @@
       <c r="AQ237" s="7"/>
       <c r="AR237" s="7"/>
     </row>
-    <row r="238" spans="1:45">
-      <c r="A238" s="20"/>
+    <row r="238" spans="1:45" x14ac:dyDescent="0.3">
+      <c r="A238" s="23"/>
       <c r="B238" s="7"/>
       <c r="C238" s="7"/>
       <c r="D238" s="7"/>
@@ -24195,8 +24229,8 @@
       <c r="AQ238" s="7"/>
       <c r="AR238" s="7"/>
     </row>
-    <row r="239" spans="1:45">
-      <c r="A239" s="20"/>
+    <row r="239" spans="1:45" x14ac:dyDescent="0.3">
+      <c r="A239" s="23"/>
       <c r="B239" s="2" t="s">
         <v>2266</v>
       </c>
@@ -24261,8 +24295,8 @@
       <c r="AQ239" s="7"/>
       <c r="AR239" s="7"/>
     </row>
-    <row r="240" spans="1:45">
-      <c r="A240" s="20"/>
+    <row r="240" spans="1:45" x14ac:dyDescent="0.3">
+      <c r="A240" s="23"/>
       <c r="B240" s="7"/>
       <c r="C240" s="7"/>
       <c r="D240" s="7"/>
@@ -24307,8 +24341,8 @@
       <c r="AQ240" s="7"/>
       <c r="AR240" s="7"/>
     </row>
-    <row r="241" spans="1:44">
-      <c r="A241" s="20"/>
+    <row r="241" spans="1:44" x14ac:dyDescent="0.3">
+      <c r="A241" s="23"/>
       <c r="B241" s="2" t="s">
         <v>2276</v>
       </c>
@@ -24387,8 +24421,8 @@
       <c r="AQ241" s="7"/>
       <c r="AR241" s="7"/>
     </row>
-    <row r="242" spans="1:44">
-      <c r="A242" s="20"/>
+    <row r="242" spans="1:44" x14ac:dyDescent="0.3">
+      <c r="A242" s="23"/>
       <c r="B242" s="7"/>
       <c r="C242" s="7"/>
       <c r="D242" s="7"/>
@@ -24433,8 +24467,8 @@
       <c r="AQ242" s="7"/>
       <c r="AR242" s="7"/>
     </row>
-    <row r="243" spans="1:44">
-      <c r="A243" s="20"/>
+    <row r="243" spans="1:44" x14ac:dyDescent="0.3">
+      <c r="A243" s="23"/>
       <c r="B243" s="2" t="s">
         <v>2293</v>
       </c>
@@ -24515,8 +24549,8 @@
       <c r="AQ243" s="7"/>
       <c r="AR243" s="7"/>
     </row>
-    <row r="244" spans="1:44">
-      <c r="A244" s="20"/>
+    <row r="244" spans="1:44" x14ac:dyDescent="0.3">
+      <c r="A244" s="23"/>
       <c r="B244" s="7"/>
       <c r="C244" s="7"/>
       <c r="D244" s="7"/>
@@ -24561,8 +24595,8 @@
       <c r="AQ244" s="7"/>
       <c r="AR244" s="7"/>
     </row>
-    <row r="245" spans="1:44">
-      <c r="A245" s="20"/>
+    <row r="245" spans="1:44" x14ac:dyDescent="0.3">
+      <c r="A245" s="23"/>
       <c r="B245" s="1" t="s">
         <v>2311</v>
       </c>
@@ -24637,8 +24671,8 @@
       <c r="AQ245" s="7"/>
       <c r="AR245" s="7"/>
     </row>
-    <row r="246" spans="1:44">
-      <c r="A246" s="20"/>
+    <row r="246" spans="1:44" x14ac:dyDescent="0.3">
+      <c r="A246" s="23"/>
       <c r="B246" s="7"/>
       <c r="C246" s="7"/>
       <c r="D246" s="7"/>
@@ -24683,8 +24717,8 @@
       <c r="AQ246" s="7"/>
       <c r="AR246" s="7"/>
     </row>
-    <row r="247" spans="1:44">
-      <c r="A247" s="20"/>
+    <row r="247" spans="1:44" x14ac:dyDescent="0.3">
+      <c r="A247" s="23"/>
       <c r="B247" s="2" t="s">
         <v>2326</v>
       </c>
@@ -24743,8 +24777,8 @@
       <c r="AQ247" s="7"/>
       <c r="AR247" s="7"/>
     </row>
-    <row r="248" spans="1:44">
-      <c r="A248" s="20"/>
+    <row r="248" spans="1:44" x14ac:dyDescent="0.3">
+      <c r="A248" s="23"/>
       <c r="B248" s="7"/>
       <c r="C248" s="7"/>
       <c r="D248" s="7"/>
@@ -24789,8 +24823,8 @@
       <c r="AQ248" s="7"/>
       <c r="AR248" s="7"/>
     </row>
-    <row r="249" spans="1:44">
-      <c r="A249" s="20"/>
+    <row r="249" spans="1:44" x14ac:dyDescent="0.3">
+      <c r="A249" s="23"/>
       <c r="B249" s="2" t="s">
         <v>2333</v>
       </c>
@@ -24905,8 +24939,8 @@
       <c r="AQ249" s="7"/>
       <c r="AR249" s="7"/>
     </row>
-    <row r="250" spans="1:44">
-      <c r="A250" s="20"/>
+    <row r="250" spans="1:44" x14ac:dyDescent="0.3">
+      <c r="A250" s="23"/>
       <c r="B250" s="7"/>
       <c r="C250" s="7"/>
       <c r="D250" s="7"/>
@@ -24951,7 +24985,7 @@
       <c r="AQ250" s="7"/>
       <c r="AR250" s="7"/>
     </row>
-    <row r="251" spans="1:44">
+    <row r="251" spans="1:44" x14ac:dyDescent="0.3">
       <c r="B251" t="s">
         <v>159</v>
       </c>
@@ -25075,12 +25109,12 @@
     </row>
   </sheetData>
   <mergeCells count="6">
-    <mergeCell ref="A211:A250"/>
+    <mergeCell ref="A210:A250"/>
     <mergeCell ref="A1:A40"/>
-    <mergeCell ref="A43:A82"/>
-    <mergeCell ref="A169:A208"/>
-    <mergeCell ref="A85:A124"/>
-    <mergeCell ref="A127:A166"/>
+    <mergeCell ref="A42:A82"/>
+    <mergeCell ref="A84:A124"/>
+    <mergeCell ref="A126:A166"/>
+    <mergeCell ref="A168:A208"/>
   </mergeCells>
   <phoneticPr fontId="18" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -25092,125 +25126,125 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:X29"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K34" sqref="K34"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="U25" sqref="U25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5"/>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:24">
+    <row r="1" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A1" s="9"/>
-      <c r="B1" s="20" t="s">
+      <c r="B1" s="23" t="s">
+        <v>2484</v>
+      </c>
+      <c r="C1" s="23"/>
+      <c r="D1" s="23"/>
+      <c r="E1" s="23"/>
+      <c r="F1" s="23"/>
+      <c r="G1" s="23"/>
+      <c r="H1" s="23"/>
+      <c r="I1" s="23"/>
+      <c r="J1" s="23"/>
+      <c r="K1" s="12"/>
+      <c r="L1" s="23" t="s">
         <v>2485</v>
       </c>
-      <c r="C1" s="20"/>
-      <c r="D1" s="20"/>
-      <c r="E1" s="20"/>
-      <c r="F1" s="20"/>
-      <c r="G1" s="20"/>
-      <c r="H1" s="20"/>
-      <c r="I1" s="20"/>
-      <c r="J1" s="20"/>
-      <c r="K1" s="12"/>
-      <c r="L1" s="20" t="s">
+      <c r="M1" s="23"/>
+      <c r="N1" s="23"/>
+      <c r="O1" s="23"/>
+      <c r="P1" s="23"/>
+      <c r="Q1" s="12"/>
+      <c r="R1" s="23" t="s">
         <v>2486</v>
       </c>
-      <c r="M1" s="20"/>
-      <c r="N1" s="20"/>
-      <c r="O1" s="20"/>
-      <c r="P1" s="20"/>
-      <c r="Q1" s="12"/>
-      <c r="R1" s="20" t="s">
+      <c r="S1" s="23"/>
+      <c r="T1" s="23"/>
+      <c r="U1" s="23"/>
+      <c r="V1" s="23"/>
+      <c r="W1" s="23"/>
+      <c r="X1" s="23"/>
+    </row>
+    <row r="2" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A2" s="9"/>
+      <c r="B2" s="20" t="s">
         <v>2487</v>
       </c>
-      <c r="S1" s="20"/>
-      <c r="T1" s="20"/>
-      <c r="U1" s="20"/>
-      <c r="V1" s="20"/>
-      <c r="W1" s="20"/>
-      <c r="X1" s="20"/>
-    </row>
-    <row r="2" spans="1:24">
-      <c r="A2" s="9"/>
-      <c r="B2" s="21" t="s">
+      <c r="C2" s="13" t="s">
         <v>2488</v>
       </c>
-      <c r="C2" s="13" t="s">
+      <c r="D2" s="21" t="s">
         <v>2489</v>
       </c>
-      <c r="D2" s="13" t="s">
+      <c r="E2" s="13" t="s">
         <v>2490</v>
       </c>
-      <c r="E2" s="13" t="s">
+      <c r="F2" s="13" t="s">
         <v>2491</v>
       </c>
-      <c r="F2" s="13" t="s">
+      <c r="G2" s="21" t="s">
+        <v>2563</v>
+      </c>
+      <c r="H2" s="13" t="s">
         <v>2492</v>
       </c>
-      <c r="G2" s="13" t="s">
-        <v>2564</v>
-      </c>
-      <c r="H2" s="13" t="s">
+      <c r="I2" s="13" t="s">
         <v>2493</v>
       </c>
-      <c r="I2" s="13" t="s">
+      <c r="J2" s="13" t="s">
         <v>2494</v>
       </c>
-      <c r="J2" s="13" t="s">
+      <c r="K2" s="12"/>
+      <c r="L2" s="20" t="s">
         <v>2495</v>
       </c>
-      <c r="K2" s="12"/>
-      <c r="L2" s="21" t="s">
+      <c r="M2" s="13" t="s">
         <v>2496</v>
       </c>
-      <c r="M2" s="13" t="s">
+      <c r="N2" s="13" t="s">
         <v>2497</v>
       </c>
-      <c r="N2" s="13" t="s">
+      <c r="O2" s="21" t="s">
         <v>2498</v>
       </c>
-      <c r="O2" s="13" t="s">
+      <c r="P2" s="20" t="s">
         <v>2499</v>
-      </c>
-      <c r="P2" s="21" t="s">
-        <v>2500</v>
       </c>
       <c r="Q2" s="12"/>
       <c r="R2" s="13" t="s">
+        <v>2500</v>
+      </c>
+      <c r="S2" s="13" t="s">
         <v>2501</v>
       </c>
-      <c r="S2" s="13" t="s">
+      <c r="T2" s="13" t="s">
         <v>2502</v>
       </c>
-      <c r="T2" s="13" t="s">
+      <c r="U2" s="13" t="s">
         <v>2503</v>
       </c>
-      <c r="U2" s="13" t="s">
+      <c r="V2" s="13" t="s">
         <v>2504</v>
       </c>
-      <c r="V2" s="13" t="s">
+      <c r="W2" s="13" t="s">
         <v>2505</v>
       </c>
-      <c r="W2" s="13" t="s">
+      <c r="X2" s="13" t="s">
         <v>2506</v>
       </c>
-      <c r="X2" s="13" t="s">
+    </row>
+    <row r="3" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A3" s="20" t="s">
         <v>2507</v>
-      </c>
-    </row>
-    <row r="3" spans="1:24">
-      <c r="A3" s="21" t="s">
-        <v>2508</v>
       </c>
       <c r="B3" s="14"/>
       <c r="C3" s="15" t="s">
-        <v>2437</v>
+        <v>2436</v>
       </c>
       <c r="D3" s="14"/>
       <c r="E3" s="14"/>
       <c r="F3" s="16"/>
       <c r="G3" s="15" t="s">
-        <v>2443</v>
+        <v>2442</v>
       </c>
       <c r="H3" s="14"/>
       <c r="I3" s="14"/>
@@ -25218,7 +25252,7 @@
       <c r="K3" s="12"/>
       <c r="L3" s="14"/>
       <c r="M3" s="15" t="s">
-        <v>2458</v>
+        <v>2457</v>
       </c>
       <c r="N3" s="14"/>
       <c r="O3" s="14"/>
@@ -25230,13 +25264,13 @@
       <c r="U3" s="14"/>
       <c r="V3" s="14"/>
       <c r="W3" s="15" t="s">
-        <v>2476</v>
+        <v>2475</v>
       </c>
       <c r="X3" s="14"/>
     </row>
-    <row r="4" spans="1:24">
+    <row r="4" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A4" s="13" t="s">
-        <v>2509</v>
+        <v>2508</v>
       </c>
       <c r="B4" s="14"/>
       <c r="C4" s="14"/>
@@ -25249,7 +25283,7 @@
       <c r="J4" s="14"/>
       <c r="K4" s="12"/>
       <c r="L4" s="15" t="s">
-        <v>2535</v>
+        <v>2534</v>
       </c>
       <c r="M4" s="14"/>
       <c r="N4" s="14"/>
@@ -25264,12 +25298,12 @@
       <c r="W4" s="14"/>
       <c r="X4" s="14"/>
     </row>
-    <row r="5" spans="1:24">
+    <row r="5" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A5" s="13" t="s">
-        <v>2510</v>
+        <v>2509</v>
       </c>
       <c r="B5" s="15" t="s">
-        <v>2435</v>
+        <v>2434</v>
       </c>
       <c r="C5" s="14"/>
       <c r="D5" s="14"/>
@@ -25281,7 +25315,7 @@
       <c r="J5" s="14"/>
       <c r="K5" s="12"/>
       <c r="L5" s="15" t="s">
-        <v>2452</v>
+        <v>2451</v>
       </c>
       <c r="M5" s="14"/>
       <c r="N5" s="14"/>
@@ -25296,15 +25330,15 @@
       <c r="W5" s="14"/>
       <c r="X5" s="14"/>
     </row>
-    <row r="6" spans="1:24">
+    <row r="6" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A6" s="13" t="s">
-        <v>2565</v>
+        <v>2564</v>
       </c>
       <c r="B6" s="14"/>
       <c r="C6" s="14"/>
       <c r="D6" s="14"/>
       <c r="E6" s="15" t="s">
-        <v>2440</v>
+        <v>2439</v>
       </c>
       <c r="F6" s="14"/>
       <c r="G6" s="14"/>
@@ -25319,23 +25353,23 @@
       <c r="P6" s="14"/>
       <c r="Q6" s="12"/>
       <c r="R6" s="15" t="s">
-        <v>2480</v>
+        <v>2479</v>
       </c>
       <c r="S6" s="14"/>
       <c r="T6" s="14"/>
       <c r="U6" s="14"/>
       <c r="V6" s="15" t="s">
-        <v>2478</v>
+        <v>2477</v>
       </c>
       <c r="W6" s="14"/>
       <c r="X6" s="14"/>
     </row>
-    <row r="7" spans="1:24">
-      <c r="A7" s="13" t="s">
-        <v>2511</v>
+    <row r="7" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A7" s="21" t="s">
+        <v>2510</v>
       </c>
       <c r="B7" s="17" t="s">
-        <v>2439</v>
+        <v>2438</v>
       </c>
       <c r="C7" s="14"/>
       <c r="D7" s="14"/>
@@ -25360,14 +25394,14 @@
       <c r="W7" s="14"/>
       <c r="X7" s="14"/>
     </row>
-    <row r="8" spans="1:24">
+    <row r="8" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A8" s="13" t="s">
-        <v>2512</v>
+        <v>2511</v>
       </c>
       <c r="B8" s="14"/>
       <c r="C8" s="14"/>
       <c r="D8" s="15" t="s">
-        <v>2442</v>
+        <v>2441</v>
       </c>
       <c r="E8" s="14"/>
       <c r="F8" s="14"/>
@@ -25381,7 +25415,7 @@
       <c r="N8" s="14"/>
       <c r="O8" s="14"/>
       <c r="P8" s="15" t="s">
-        <v>2448</v>
+        <v>2447</v>
       </c>
       <c r="Q8" s="12"/>
       <c r="R8" s="14"/>
@@ -25392,9 +25426,9 @@
       <c r="W8" s="14"/>
       <c r="X8" s="14"/>
     </row>
-    <row r="9" spans="1:24">
-      <c r="A9" s="13" t="s">
-        <v>2513</v>
+    <row r="9" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A9" s="21" t="s">
+        <v>2512</v>
       </c>
       <c r="B9" s="14"/>
       <c r="C9" s="14"/>
@@ -25409,7 +25443,7 @@
       <c r="L9" s="14"/>
       <c r="M9" s="9"/>
       <c r="N9" s="15" t="s">
-        <v>2447</v>
+        <v>2446</v>
       </c>
       <c r="O9" s="14"/>
       <c r="P9" s="14"/>
@@ -25422,15 +25456,15 @@
       <c r="W9" s="9"/>
       <c r="X9" s="9"/>
     </row>
-    <row r="10" spans="1:24">
-      <c r="A10" s="21" t="s">
-        <v>2514</v>
+    <row r="10" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A10" s="20" t="s">
+        <v>2513</v>
       </c>
       <c r="B10" s="14"/>
       <c r="C10" s="14"/>
       <c r="D10" s="14"/>
       <c r="E10" s="15" t="s">
-        <v>2436</v>
+        <v>2435</v>
       </c>
       <c r="F10" s="14"/>
       <c r="G10" s="14"/>
@@ -25440,30 +25474,30 @@
       <c r="K10" s="12"/>
       <c r="L10" s="14"/>
       <c r="M10" s="15" t="s">
-        <v>2463</v>
+        <v>2462</v>
       </c>
       <c r="N10" s="14"/>
       <c r="O10" s="15" t="s">
-        <v>2461</v>
+        <v>2460</v>
       </c>
       <c r="P10" s="14"/>
       <c r="Q10" s="12"/>
       <c r="R10" s="14"/>
       <c r="S10" s="14"/>
       <c r="T10" s="15" t="s">
-        <v>2467</v>
+        <v>2466</v>
       </c>
       <c r="U10" s="14"/>
       <c r="V10" s="14"/>
       <c r="W10" s="14"/>
       <c r="X10" s="14"/>
     </row>
-    <row r="11" spans="1:24">
-      <c r="A11" s="13" t="s">
-        <v>2515</v>
+    <row r="11" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A11" s="21" t="s">
+        <v>2514</v>
       </c>
       <c r="B11" s="15" t="s">
-        <v>2444</v>
+        <v>2443</v>
       </c>
       <c r="C11" s="14"/>
       <c r="D11" s="14"/>
@@ -25488,9 +25522,9 @@
       <c r="W11" s="14"/>
       <c r="X11" s="14"/>
     </row>
-    <row r="12" spans="1:24">
-      <c r="A12" s="13" t="s">
-        <v>2516</v>
+    <row r="12" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A12" s="21" t="s">
+        <v>2515</v>
       </c>
       <c r="B12" s="14"/>
       <c r="C12" s="14"/>
@@ -25509,7 +25543,7 @@
       <c r="P12" s="14"/>
       <c r="Q12" s="12"/>
       <c r="R12" s="15" t="s">
-        <v>2465</v>
+        <v>2464</v>
       </c>
       <c r="S12" s="9"/>
       <c r="T12" s="9"/>
@@ -25518,16 +25552,16 @@
       <c r="W12" s="9"/>
       <c r="X12" s="9"/>
     </row>
-    <row r="13" spans="1:24">
+    <row r="13" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A13" s="13" t="s">
-        <v>2517</v>
+        <v>2516</v>
       </c>
       <c r="B13" s="14"/>
       <c r="C13" s="14"/>
       <c r="D13" s="14"/>
       <c r="E13" s="14"/>
       <c r="F13" s="15" t="s">
-        <v>2536</v>
+        <v>2535</v>
       </c>
       <c r="G13" s="14"/>
       <c r="H13" s="14"/>
@@ -25548,9 +25582,9 @@
       <c r="W13" s="14"/>
       <c r="X13" s="14"/>
     </row>
-    <row r="14" spans="1:24">
-      <c r="A14" s="13" t="s">
-        <v>2518</v>
+    <row r="14" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A14" s="21" t="s">
+        <v>2517</v>
       </c>
       <c r="B14" s="14"/>
       <c r="C14" s="14"/>
@@ -25563,7 +25597,7 @@
       <c r="J14" s="14"/>
       <c r="K14" s="12"/>
       <c r="L14" s="15" t="s">
-        <v>2483</v>
+        <v>2482</v>
       </c>
       <c r="M14" s="9"/>
       <c r="N14" s="14"/>
@@ -25578,12 +25612,12 @@
       <c r="W14" s="9"/>
       <c r="X14" s="9"/>
     </row>
-    <row r="15" spans="1:24">
+    <row r="15" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A15" s="13" t="s">
-        <v>2519</v>
+        <v>2518</v>
       </c>
       <c r="B15" s="15" t="s">
-        <v>2446</v>
+        <v>2445</v>
       </c>
       <c r="C15" s="14"/>
       <c r="D15" s="14"/>
@@ -25597,7 +25631,7 @@
       <c r="L15" s="14"/>
       <c r="M15" s="14"/>
       <c r="N15" s="15" t="s">
-        <v>2464</v>
+        <v>2463</v>
       </c>
       <c r="O15" s="14"/>
       <c r="P15" s="14"/>
@@ -25610,9 +25644,9 @@
       <c r="W15" s="14"/>
       <c r="X15" s="14"/>
     </row>
-    <row r="16" spans="1:24">
-      <c r="A16" s="13" t="s">
-        <v>2520</v>
+    <row r="16" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A16" s="21" t="s">
+        <v>2519</v>
       </c>
       <c r="B16" s="14"/>
       <c r="C16" s="14"/>
@@ -25629,7 +25663,7 @@
       <c r="N16" s="14"/>
       <c r="O16" s="14"/>
       <c r="P16" s="15" t="s">
-        <v>2457</v>
+        <v>2456</v>
       </c>
       <c r="Q16" s="12"/>
       <c r="R16" s="14"/>
@@ -25640,9 +25674,9 @@
       <c r="W16" s="14"/>
       <c r="X16" s="14"/>
     </row>
-    <row r="17" spans="1:24">
+    <row r="17" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A17" s="13" t="s">
-        <v>2521</v>
+        <v>2520</v>
       </c>
       <c r="B17" s="14"/>
       <c r="C17" s="14"/>
@@ -25657,11 +25691,11 @@
       <c r="L17" s="14"/>
       <c r="M17" s="14"/>
       <c r="N17" s="15" t="s">
-        <v>2449</v>
+        <v>2448</v>
       </c>
       <c r="O17" s="14"/>
       <c r="P17" s="15" t="s">
-        <v>2456</v>
+        <v>2455</v>
       </c>
       <c r="Q17" s="12"/>
       <c r="R17" s="14"/>
@@ -25672,9 +25706,9 @@
       <c r="W17" s="14"/>
       <c r="X17" s="14"/>
     </row>
-    <row r="18" spans="1:24">
-      <c r="A18" s="21" t="s">
-        <v>2522</v>
+    <row r="18" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A18" s="20" t="s">
+        <v>2521</v>
       </c>
       <c r="B18" s="14"/>
       <c r="C18" s="14"/>
@@ -25688,10 +25722,10 @@
       <c r="K18" s="12"/>
       <c r="L18" s="14"/>
       <c r="M18" s="15" t="s">
-        <v>2460</v>
+        <v>2459</v>
       </c>
       <c r="N18" s="15" t="s">
-        <v>2462</v>
+        <v>2461</v>
       </c>
       <c r="O18" s="14"/>
       <c r="P18" s="14"/>
@@ -25699,22 +25733,22 @@
       <c r="R18" s="14"/>
       <c r="S18" s="14"/>
       <c r="T18" s="15" t="s">
-        <v>2473</v>
+        <v>2472</v>
       </c>
       <c r="U18" s="14"/>
       <c r="V18" s="14"/>
       <c r="W18" s="14"/>
       <c r="X18" s="15" t="s">
-        <v>2474</v>
-      </c>
-    </row>
-    <row r="19" spans="1:24">
-      <c r="A19" s="21" t="s">
-        <v>2523</v>
+        <v>2473</v>
+      </c>
+    </row>
+    <row r="19" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A19" s="20" t="s">
+        <v>2522</v>
       </c>
       <c r="B19" s="14"/>
       <c r="C19" s="15" t="s">
-        <v>2438</v>
+        <v>2437</v>
       </c>
       <c r="D19" s="14"/>
       <c r="E19" s="14"/>
@@ -25733,23 +25767,23 @@
       <c r="R19" s="14"/>
       <c r="S19" s="14"/>
       <c r="T19" s="15" t="s">
-        <v>2471</v>
+        <v>2470</v>
       </c>
       <c r="U19" s="15" t="s">
-        <v>2475</v>
+        <v>2474</v>
       </c>
       <c r="V19" s="16"/>
       <c r="W19" s="14"/>
       <c r="X19" s="15" t="s">
-        <v>2469</v>
-      </c>
-    </row>
-    <row r="20" spans="1:24">
-      <c r="A20" s="13" t="s">
-        <v>2524</v>
+        <v>2468</v>
+      </c>
+    </row>
+    <row r="20" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A20" s="21" t="s">
+        <v>2523</v>
       </c>
       <c r="B20" s="19" t="s">
-        <v>2428</v>
+        <v>2427</v>
       </c>
       <c r="C20" s="14"/>
       <c r="D20" s="14"/>
@@ -25774,9 +25808,9 @@
       <c r="W20" s="14"/>
       <c r="X20" s="14"/>
     </row>
-    <row r="21" spans="1:24">
+    <row r="21" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A21" s="13" t="s">
-        <v>2525</v>
+        <v>2524</v>
       </c>
       <c r="B21" s="14"/>
       <c r="C21" s="14"/>
@@ -25786,7 +25820,7 @@
       <c r="G21" s="14"/>
       <c r="H21" s="14"/>
       <c r="I21" s="17" t="s">
-        <v>2537</v>
+        <v>2536</v>
       </c>
       <c r="J21" s="14"/>
       <c r="K21" s="12"/>
@@ -25802,13 +25836,13 @@
       <c r="U21" s="14"/>
       <c r="V21" s="14"/>
       <c r="W21" s="15" t="s">
-        <v>2481</v>
+        <v>2480</v>
       </c>
       <c r="X21" s="14"/>
     </row>
-    <row r="22" spans="1:24">
-      <c r="A22" s="21" t="s">
-        <v>2526</v>
+    <row r="22" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A22" s="20" t="s">
+        <v>2525</v>
       </c>
       <c r="B22" s="14"/>
       <c r="C22" s="14"/>
@@ -25827,22 +25861,22 @@
       <c r="P22" s="14"/>
       <c r="Q22" s="12"/>
       <c r="R22" s="15" t="s">
-        <v>2466</v>
+        <v>2465</v>
       </c>
       <c r="S22" s="15" t="s">
-        <v>2534</v>
+        <v>2533</v>
       </c>
       <c r="T22" s="14"/>
       <c r="U22" s="15" t="s">
-        <v>2472</v>
+        <v>2471</v>
       </c>
       <c r="V22" s="14"/>
       <c r="W22" s="14"/>
       <c r="X22" s="14"/>
     </row>
-    <row r="23" spans="1:24">
-      <c r="A23" s="21" t="s">
-        <v>2527</v>
+    <row r="23" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A23" s="20" t="s">
+        <v>2526</v>
       </c>
       <c r="B23" s="14"/>
       <c r="C23" s="14"/>
@@ -25858,27 +25892,27 @@
       <c r="M23" s="14"/>
       <c r="N23" s="14"/>
       <c r="O23" s="15" t="s">
-        <v>2454</v>
+        <v>2453</v>
       </c>
       <c r="P23" s="14"/>
       <c r="Q23" s="12"/>
       <c r="R23" s="14"/>
       <c r="S23" s="15" t="s">
-        <v>2479</v>
+        <v>2478</v>
       </c>
       <c r="T23" s="14"/>
       <c r="U23" s="15" t="s">
-        <v>2482</v>
+        <v>2481</v>
       </c>
       <c r="V23" s="15" t="s">
-        <v>2468</v>
+        <v>2467</v>
       </c>
       <c r="W23" s="14"/>
       <c r="X23" s="14"/>
     </row>
-    <row r="24" spans="1:24">
-      <c r="A24" s="13" t="s">
-        <v>2528</v>
+    <row r="24" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A24" s="21" t="s">
+        <v>2527</v>
       </c>
       <c r="B24" s="14"/>
       <c r="C24" s="14"/>
@@ -25895,7 +25929,7 @@
       <c r="N24" s="14"/>
       <c r="O24" s="14"/>
       <c r="P24" s="15" t="s">
-        <v>2451</v>
+        <v>2450</v>
       </c>
       <c r="Q24" s="12"/>
       <c r="R24" s="14"/>
@@ -25906,9 +25940,9 @@
       <c r="W24" s="14"/>
       <c r="X24" s="14"/>
     </row>
-    <row r="25" spans="1:24">
+    <row r="25" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A25" s="13" t="s">
-        <v>2529</v>
+        <v>2528</v>
       </c>
       <c r="B25" s="14"/>
       <c r="C25" s="14"/>
@@ -25919,11 +25953,11 @@
       <c r="H25" s="14"/>
       <c r="I25" s="14"/>
       <c r="J25" s="15" t="s">
-        <v>2434</v>
+        <v>2433</v>
       </c>
       <c r="K25" s="12"/>
       <c r="L25" s="15" t="s">
-        <v>2459</v>
+        <v>2458</v>
       </c>
       <c r="M25" s="14"/>
       <c r="N25" s="14"/>
@@ -25938,9 +25972,9 @@
       <c r="W25" s="14"/>
       <c r="X25" s="14"/>
     </row>
-    <row r="26" spans="1:24">
-      <c r="A26" s="13" t="s">
-        <v>2530</v>
+    <row r="26" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A26" s="21" t="s">
+        <v>2529</v>
       </c>
       <c r="B26" s="14"/>
       <c r="C26" s="14"/>
@@ -25949,7 +25983,7 @@
       <c r="F26" s="14"/>
       <c r="G26" s="14"/>
       <c r="H26" s="19" t="s">
-        <v>2430</v>
+        <v>2429</v>
       </c>
       <c r="I26" s="14"/>
       <c r="J26" s="14"/>
@@ -25968,9 +26002,9 @@
       <c r="W26" s="14"/>
       <c r="X26" s="14"/>
     </row>
-    <row r="27" spans="1:24">
-      <c r="A27" s="13" t="s">
-        <v>2531</v>
+    <row r="27" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A27" s="22" t="s">
+        <v>2530</v>
       </c>
       <c r="B27" s="14"/>
       <c r="C27" s="14"/>
@@ -25979,7 +26013,7 @@
       <c r="F27" s="14"/>
       <c r="G27" s="14"/>
       <c r="H27" s="15" t="s">
-        <v>2429</v>
+        <v>2428</v>
       </c>
       <c r="I27" s="14"/>
       <c r="J27" s="14"/>
@@ -25998,9 +26032,9 @@
       <c r="W27" s="9"/>
       <c r="X27" s="9"/>
     </row>
-    <row r="28" spans="1:24">
-      <c r="A28" s="13" t="s">
-        <v>2532</v>
+    <row r="28" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A28" s="22" t="s">
+        <v>2531</v>
       </c>
       <c r="B28" s="14"/>
       <c r="C28" s="14"/>
@@ -26017,7 +26051,7 @@
       <c r="N28" s="14"/>
       <c r="O28" s="14"/>
       <c r="P28" s="15" t="s">
-        <v>2450</v>
+        <v>2449</v>
       </c>
       <c r="Q28" s="12"/>
       <c r="R28" s="14"/>
@@ -26028,9 +26062,9 @@
       <c r="W28" s="14"/>
       <c r="X28" s="14"/>
     </row>
-    <row r="29" spans="1:24">
-      <c r="A29" s="13" t="s">
-        <v>2533</v>
+    <row r="29" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A29" s="22" t="s">
+        <v>2532</v>
       </c>
       <c r="B29" s="14"/>
       <c r="C29" s="14"/>
@@ -26041,7 +26075,7 @@
       <c r="H29" s="14"/>
       <c r="I29" s="14"/>
       <c r="J29" s="15" t="s">
-        <v>2441</v>
+        <v>2440</v>
       </c>
       <c r="K29" s="12"/>
       <c r="L29" s="14"/>
@@ -26074,75 +26108,75 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T7"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="Q13" sqref="Q13"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K10" sqref="K10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5"/>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:20">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A1" s="13"/>
       <c r="B1" s="13" t="s">
+        <v>2537</v>
+      </c>
+      <c r="C1" s="13" t="s">
+        <v>2540</v>
+      </c>
+      <c r="D1" s="13" t="s">
         <v>2538</v>
       </c>
-      <c r="C1" s="13" t="s">
+      <c r="E1" s="13" t="s">
         <v>2541</v>
       </c>
-      <c r="D1" s="13" t="s">
+      <c r="F1" s="13" t="s">
+        <v>2542</v>
+      </c>
+      <c r="G1" s="13" t="s">
+        <v>2543</v>
+      </c>
+      <c r="H1" s="13" t="s">
         <v>2539</v>
       </c>
-      <c r="E1" s="13" t="s">
-        <v>2542</v>
-      </c>
-      <c r="F1" s="13" t="s">
-        <v>2543</v>
-      </c>
-      <c r="G1" s="13" t="s">
+      <c r="I1" s="13" t="s">
         <v>2544</v>
       </c>
-      <c r="H1" s="13" t="s">
-        <v>2540</v>
-      </c>
-      <c r="I1" s="13" t="s">
+      <c r="J1" s="13" t="s">
         <v>2545</v>
       </c>
-      <c r="J1" s="13" t="s">
+      <c r="K1" s="13" t="s">
         <v>2546</v>
       </c>
-      <c r="K1" s="13" t="s">
+      <c r="L1" s="13" t="s">
         <v>2547</v>
       </c>
-      <c r="L1" s="13" t="s">
+      <c r="M1" s="13" t="s">
         <v>2548</v>
       </c>
-      <c r="M1" s="13" t="s">
+      <c r="N1" s="13" t="s">
         <v>2549</v>
       </c>
-      <c r="N1" s="13" t="s">
+      <c r="O1" s="13" t="s">
         <v>2550</v>
       </c>
-      <c r="O1" s="13" t="s">
+      <c r="P1" s="13" t="s">
         <v>2551</v>
       </c>
-      <c r="P1" s="13" t="s">
+      <c r="Q1" s="13" t="s">
         <v>2552</v>
       </c>
-      <c r="Q1" s="13" t="s">
+      <c r="R1" s="13" t="s">
         <v>2553</v>
       </c>
-      <c r="R1" s="13" t="s">
+      <c r="S1" s="13" t="s">
         <v>2554</v>
       </c>
-      <c r="S1" s="13" t="s">
+      <c r="T1" s="13" t="s">
         <v>2555</v>
       </c>
-      <c r="T1" s="13" t="s">
+    </row>
+    <row r="2" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A2" s="13" t="s">
         <v>2556</v>
-      </c>
-    </row>
-    <row r="2" spans="1:20">
-      <c r="A2" s="13" t="s">
-        <v>2557</v>
       </c>
       <c r="B2" s="11" t="s">
         <v>2371</v>
@@ -26169,345 +26203,345 @@
         <v>2378</v>
       </c>
       <c r="J2" s="11" t="s">
+        <v>2565</v>
+      </c>
+      <c r="K2" s="11" t="s">
         <v>2379</v>
       </c>
-      <c r="K2" s="11" t="s">
+      <c r="L2" s="11" t="s">
         <v>2380</v>
       </c>
-      <c r="L2" s="11" t="s">
+      <c r="M2" s="11" t="s">
         <v>2381</v>
       </c>
-      <c r="M2" s="11" t="s">
+      <c r="N2" s="11" t="s">
         <v>2382</v>
       </c>
-      <c r="N2" s="11" t="s">
+      <c r="O2" s="11" t="s">
         <v>2383</v>
       </c>
-      <c r="O2" s="11" t="s">
+      <c r="P2" s="11" t="s">
         <v>2384</v>
       </c>
-      <c r="P2" s="11" t="s">
+      <c r="Q2" s="11" t="s">
         <v>2385</v>
       </c>
-      <c r="Q2" s="11" t="s">
+      <c r="R2" s="11" t="s">
         <v>2386</v>
       </c>
-      <c r="R2" s="11" t="s">
+      <c r="S2" s="11" t="s">
         <v>2387</v>
       </c>
-      <c r="S2" s="11" t="s">
+      <c r="T2" s="11" t="s">
         <v>2388</v>
       </c>
-      <c r="T2" s="11" t="s">
+    </row>
+    <row r="3" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A3" s="13" t="s">
+        <v>2557</v>
+      </c>
+      <c r="B3" s="11" t="s">
         <v>2389</v>
       </c>
-    </row>
-    <row r="3" spans="1:20">
-      <c r="A3" s="13" t="s">
+      <c r="C3" s="11" t="s">
+        <v>2390</v>
+      </c>
+      <c r="D3" s="11" t="s">
+        <v>2391</v>
+      </c>
+      <c r="E3" s="11" t="s">
+        <v>2392</v>
+      </c>
+      <c r="F3" s="11" t="s">
+        <v>2393</v>
+      </c>
+      <c r="G3" s="11" t="s">
+        <v>2394</v>
+      </c>
+      <c r="H3" s="11" t="s">
+        <v>2395</v>
+      </c>
+      <c r="I3" s="11" t="s">
+        <v>2396</v>
+      </c>
+      <c r="J3" s="11" t="s">
+        <v>2397</v>
+      </c>
+      <c r="K3" s="11" t="s">
+        <v>2398</v>
+      </c>
+      <c r="L3" s="11" t="s">
+        <v>2399</v>
+      </c>
+      <c r="M3" s="11" t="s">
+        <v>2400</v>
+      </c>
+      <c r="N3" s="11" t="s">
+        <v>2401</v>
+      </c>
+      <c r="O3" s="11" t="s">
+        <v>2402</v>
+      </c>
+      <c r="P3" s="11" t="s">
+        <v>2403</v>
+      </c>
+      <c r="Q3" s="11" t="s">
+        <v>2404</v>
+      </c>
+      <c r="R3" s="11" t="s">
+        <v>2405</v>
+      </c>
+      <c r="S3" s="11" t="s">
+        <v>2406</v>
+      </c>
+      <c r="T3" s="11" t="s">
+        <v>2407</v>
+      </c>
+    </row>
+    <row r="4" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A4" s="13" t="s">
         <v>2558</v>
       </c>
-      <c r="B3" s="11" t="s">
-        <v>2390</v>
-      </c>
-      <c r="C3" s="11" t="s">
-        <v>2391</v>
-      </c>
-      <c r="D3" s="11" t="s">
-        <v>2392</v>
-      </c>
-      <c r="E3" s="11" t="s">
-        <v>2393</v>
-      </c>
-      <c r="F3" s="11" t="s">
-        <v>2394</v>
-      </c>
-      <c r="G3" s="11" t="s">
-        <v>2395</v>
-      </c>
-      <c r="H3" s="11" t="s">
-        <v>2396</v>
-      </c>
-      <c r="I3" s="11" t="s">
-        <v>2397</v>
-      </c>
-      <c r="J3" s="11" t="s">
-        <v>2398</v>
-      </c>
-      <c r="K3" s="11" t="s">
-        <v>2399</v>
-      </c>
-      <c r="L3" s="11" t="s">
-        <v>2400</v>
-      </c>
-      <c r="M3" s="11" t="s">
-        <v>2401</v>
-      </c>
-      <c r="N3" s="11" t="s">
-        <v>2402</v>
-      </c>
-      <c r="O3" s="11" t="s">
-        <v>2403</v>
-      </c>
-      <c r="P3" s="11" t="s">
-        <v>2404</v>
-      </c>
-      <c r="Q3" s="11" t="s">
-        <v>2405</v>
-      </c>
-      <c r="R3" s="11" t="s">
-        <v>2406</v>
-      </c>
-      <c r="S3" s="11" t="s">
-        <v>2407</v>
-      </c>
-      <c r="T3" s="11" t="s">
+      <c r="B4" s="11" t="s">
         <v>2408</v>
       </c>
-    </row>
-    <row r="4" spans="1:20">
-      <c r="A4" s="13" t="s">
+      <c r="C4" s="11" t="s">
+        <v>2409</v>
+      </c>
+      <c r="D4" s="11" t="s">
+        <v>2410</v>
+      </c>
+      <c r="E4" s="11" t="s">
+        <v>2411</v>
+      </c>
+      <c r="F4" s="11" t="s">
+        <v>2412</v>
+      </c>
+      <c r="G4" s="11" t="s">
+        <v>2413</v>
+      </c>
+      <c r="H4" s="11" t="s">
+        <v>2414</v>
+      </c>
+      <c r="I4" s="11" t="s">
+        <v>2415</v>
+      </c>
+      <c r="J4" s="11" t="s">
+        <v>2416</v>
+      </c>
+      <c r="K4" s="11" t="s">
+        <v>2417</v>
+      </c>
+      <c r="L4" s="11" t="s">
+        <v>2418</v>
+      </c>
+      <c r="M4" s="11" t="s">
+        <v>2419</v>
+      </c>
+      <c r="N4" s="11" t="s">
+        <v>2420</v>
+      </c>
+      <c r="O4" s="11" t="s">
+        <v>2421</v>
+      </c>
+      <c r="P4" s="11" t="s">
+        <v>2422</v>
+      </c>
+      <c r="Q4" s="11" t="s">
+        <v>2423</v>
+      </c>
+      <c r="R4" s="11" t="s">
+        <v>2424</v>
+      </c>
+      <c r="S4" s="11" t="s">
+        <v>2425</v>
+      </c>
+      <c r="T4" s="11" t="s">
+        <v>2426</v>
+      </c>
+    </row>
+    <row r="5" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A5" s="13" t="s">
         <v>2559</v>
       </c>
-      <c r="B4" s="11" t="s">
-        <v>2409</v>
-      </c>
-      <c r="C4" s="11" t="s">
-        <v>2410</v>
-      </c>
-      <c r="D4" s="11" t="s">
-        <v>2411</v>
-      </c>
-      <c r="E4" s="11" t="s">
-        <v>2412</v>
-      </c>
-      <c r="F4" s="11" t="s">
-        <v>2413</v>
-      </c>
-      <c r="G4" s="11" t="s">
-        <v>2414</v>
-      </c>
-      <c r="H4" s="11" t="s">
-        <v>2415</v>
-      </c>
-      <c r="I4" s="11" t="s">
-        <v>2416</v>
-      </c>
-      <c r="J4" s="11" t="s">
-        <v>2417</v>
-      </c>
-      <c r="K4" s="11" t="s">
-        <v>2418</v>
-      </c>
-      <c r="L4" s="11" t="s">
-        <v>2419</v>
-      </c>
-      <c r="M4" s="11" t="s">
-        <v>2420</v>
-      </c>
-      <c r="N4" s="11" t="s">
-        <v>2421</v>
-      </c>
-      <c r="O4" s="11" t="s">
-        <v>2422</v>
-      </c>
-      <c r="P4" s="11" t="s">
-        <v>2423</v>
-      </c>
-      <c r="Q4" s="11" t="s">
-        <v>2424</v>
-      </c>
-      <c r="R4" s="11" t="s">
-        <v>2425</v>
-      </c>
-      <c r="S4" s="11" t="s">
-        <v>2426</v>
-      </c>
-      <c r="T4" s="11" t="s">
+      <c r="B5" s="11" t="s">
         <v>2427</v>
       </c>
-    </row>
-    <row r="5" spans="1:20">
-      <c r="A5" s="13" t="s">
+      <c r="C5" s="11" t="s">
+        <v>2428</v>
+      </c>
+      <c r="D5" s="11" t="s">
+        <v>2429</v>
+      </c>
+      <c r="E5" s="11" t="s">
+        <v>2430</v>
+      </c>
+      <c r="F5" s="11" t="s">
+        <v>2431</v>
+      </c>
+      <c r="G5" s="11" t="s">
+        <v>2432</v>
+      </c>
+      <c r="H5" s="11" t="s">
+        <v>2433</v>
+      </c>
+      <c r="I5" s="11" t="s">
+        <v>2434</v>
+      </c>
+      <c r="J5" s="11" t="s">
+        <v>2436</v>
+      </c>
+      <c r="K5" s="11" t="s">
+        <v>2435</v>
+      </c>
+      <c r="L5" s="11" t="s">
+        <v>2437</v>
+      </c>
+      <c r="M5" s="11" t="s">
+        <v>2438</v>
+      </c>
+      <c r="N5" s="11" t="s">
+        <v>2439</v>
+      </c>
+      <c r="O5" s="11" t="s">
+        <v>2440</v>
+      </c>
+      <c r="P5" s="11" t="s">
+        <v>2441</v>
+      </c>
+      <c r="Q5" s="11" t="s">
+        <v>2442</v>
+      </c>
+      <c r="R5" s="11" t="s">
+        <v>2443</v>
+      </c>
+      <c r="S5" s="11" t="s">
+        <v>2444</v>
+      </c>
+      <c r="T5" s="11" t="s">
+        <v>2445</v>
+      </c>
+    </row>
+    <row r="6" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A6" s="13" t="s">
         <v>2560</v>
       </c>
-      <c r="B5" s="11" t="s">
-        <v>2428</v>
-      </c>
-      <c r="C5" s="11" t="s">
-        <v>2429</v>
-      </c>
-      <c r="D5" s="11" t="s">
-        <v>2430</v>
-      </c>
-      <c r="E5" s="11" t="s">
-        <v>2431</v>
-      </c>
-      <c r="F5" s="11" t="s">
-        <v>2432</v>
-      </c>
-      <c r="G5" s="11" t="s">
-        <v>2433</v>
-      </c>
-      <c r="H5" s="11" t="s">
-        <v>2434</v>
-      </c>
-      <c r="I5" s="11" t="s">
-        <v>2435</v>
-      </c>
-      <c r="J5" s="11" t="s">
-        <v>2437</v>
-      </c>
-      <c r="K5" s="11" t="s">
-        <v>2436</v>
-      </c>
-      <c r="L5" s="11" t="s">
-        <v>2438</v>
-      </c>
-      <c r="M5" s="11" t="s">
-        <v>2439</v>
-      </c>
-      <c r="N5" s="11" t="s">
-        <v>2440</v>
-      </c>
-      <c r="O5" s="11" t="s">
-        <v>2441</v>
-      </c>
-      <c r="P5" s="11" t="s">
-        <v>2442</v>
-      </c>
-      <c r="Q5" s="11" t="s">
-        <v>2443</v>
-      </c>
-      <c r="R5" s="11" t="s">
-        <v>2444</v>
-      </c>
-      <c r="S5" s="11" t="s">
-        <v>2445</v>
-      </c>
-      <c r="T5" s="11" t="s">
+      <c r="B6" s="11" t="s">
         <v>2446</v>
       </c>
-    </row>
-    <row r="6" spans="1:20">
-      <c r="A6" s="13" t="s">
+      <c r="C6" s="11" t="s">
+        <v>2447</v>
+      </c>
+      <c r="D6" s="11" t="s">
+        <v>2450</v>
+      </c>
+      <c r="E6" s="11" t="s">
+        <v>2482</v>
+      </c>
+      <c r="F6" s="11" t="s">
+        <v>2448</v>
+      </c>
+      <c r="G6" s="11" t="s">
+        <v>2449</v>
+      </c>
+      <c r="H6" s="11" t="s">
+        <v>2451</v>
+      </c>
+      <c r="I6" s="11" t="s">
+        <v>2452</v>
+      </c>
+      <c r="J6" s="11" t="s">
+        <v>2453</v>
+      </c>
+      <c r="K6" s="11" t="s">
+        <v>2454</v>
+      </c>
+      <c r="L6" s="11" t="s">
+        <v>2455</v>
+      </c>
+      <c r="M6" s="11" t="s">
+        <v>2456</v>
+      </c>
+      <c r="N6" s="11" t="s">
+        <v>2457</v>
+      </c>
+      <c r="O6" s="11" t="s">
+        <v>2458</v>
+      </c>
+      <c r="P6" s="11" t="s">
+        <v>2459</v>
+      </c>
+      <c r="Q6" s="11" t="s">
+        <v>2460</v>
+      </c>
+      <c r="R6" s="11" t="s">
+        <v>2461</v>
+      </c>
+      <c r="S6" s="11" t="s">
+        <v>2462</v>
+      </c>
+      <c r="T6" s="11" t="s">
+        <v>2463</v>
+      </c>
+    </row>
+    <row r="7" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A7" s="13" t="s">
         <v>2561</v>
       </c>
-      <c r="B6" s="11" t="s">
-        <v>2447</v>
-      </c>
-      <c r="C6" s="11" t="s">
-        <v>2448</v>
-      </c>
-      <c r="D6" s="11" t="s">
-        <v>2451</v>
-      </c>
-      <c r="E6" s="11" t="s">
-        <v>2483</v>
-      </c>
-      <c r="F6" s="11" t="s">
-        <v>2449</v>
-      </c>
-      <c r="G6" s="11" t="s">
-        <v>2450</v>
-      </c>
-      <c r="H6" s="11" t="s">
-        <v>2452</v>
-      </c>
-      <c r="I6" s="11" t="s">
-        <v>2453</v>
-      </c>
-      <c r="J6" s="11" t="s">
-        <v>2454</v>
-      </c>
-      <c r="K6" s="11" t="s">
-        <v>2455</v>
-      </c>
-      <c r="L6" s="11" t="s">
-        <v>2456</v>
-      </c>
-      <c r="M6" s="11" t="s">
-        <v>2457</v>
-      </c>
-      <c r="N6" s="11" t="s">
-        <v>2458</v>
-      </c>
-      <c r="O6" s="11" t="s">
-        <v>2459</v>
-      </c>
-      <c r="P6" s="11" t="s">
-        <v>2460</v>
-      </c>
-      <c r="Q6" s="11" t="s">
-        <v>2461</v>
-      </c>
-      <c r="R6" s="11" t="s">
-        <v>2462</v>
-      </c>
-      <c r="S6" s="11" t="s">
-        <v>2463</v>
-      </c>
-      <c r="T6" s="11" t="s">
+      <c r="B7" s="11" t="s">
         <v>2464</v>
       </c>
-    </row>
-    <row r="7" spans="1:20">
-      <c r="A7" s="13" t="s">
-        <v>2562</v>
-      </c>
-      <c r="B7" s="11" t="s">
+      <c r="C7" s="11" t="s">
         <v>2465</v>
       </c>
-      <c r="C7" s="11" t="s">
+      <c r="D7" s="11" t="s">
         <v>2466</v>
-      </c>
-      <c r="D7" s="11" t="s">
-        <v>2467</v>
       </c>
       <c r="E7" s="11" t="s">
         <v>2102</v>
       </c>
       <c r="F7" s="11" t="s">
+        <v>2468</v>
+      </c>
+      <c r="G7" s="11" t="s">
         <v>2469</v>
       </c>
-      <c r="G7" s="11" t="s">
+      <c r="H7" s="11" t="s">
         <v>2470</v>
       </c>
-      <c r="H7" s="11" t="s">
+      <c r="I7" s="11" t="s">
         <v>2471</v>
-      </c>
-      <c r="I7" s="11" t="s">
-        <v>2472</v>
       </c>
       <c r="J7" s="10"/>
       <c r="K7" s="11" t="s">
+        <v>2472</v>
+      </c>
+      <c r="L7" s="11" t="s">
         <v>2473</v>
       </c>
-      <c r="L7" s="11" t="s">
+      <c r="M7" s="11" t="s">
         <v>2474</v>
       </c>
-      <c r="M7" s="11" t="s">
+      <c r="N7" s="11" t="s">
         <v>2475</v>
       </c>
-      <c r="N7" s="11" t="s">
+      <c r="O7" s="11" t="s">
         <v>2476</v>
       </c>
-      <c r="O7" s="11" t="s">
+      <c r="P7" s="11" t="s">
         <v>2477</v>
       </c>
-      <c r="P7" s="11" t="s">
+      <c r="Q7" s="11" t="s">
         <v>2478</v>
       </c>
-      <c r="Q7" s="11" t="s">
+      <c r="R7" s="11" t="s">
         <v>2479</v>
       </c>
-      <c r="R7" s="11" t="s">
+      <c r="S7" s="11" t="s">
         <v>2480</v>
       </c>
-      <c r="S7" s="11" t="s">
+      <c r="T7" s="11" t="s">
         <v>2481</v>
-      </c>
-      <c r="T7" s="11" t="s">
-        <v>2482</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add new version of basis characters
</commit_message>
<xml_diff>
--- a/output/labels-map(ANSI).xlsx
+++ b/output/labels-map(ANSI).xlsx
@@ -25127,7 +25127,7 @@
   <dimension ref="A1:X29"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="U25" sqref="U25"/>
+      <selection activeCell="P35" sqref="P35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -26109,7 +26109,7 @@
   <dimension ref="A1:T7"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K10" sqref="K10"/>
+      <selection activeCell="J20" sqref="J20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>

</xml_diff>